<commit_message>
Minor update to plan
update to sprint plan
</commit_message>
<xml_diff>
--- a/TeamNick_Jeremy_AmieReport.xlsx
+++ b/TeamNick_Jeremy_AmieReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="21360" windowHeight="14400" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="220" yWindow="220" windowWidth="21360" windowHeight="14400" tabRatio="500" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="274">
+  <si>
+    <t>Modify program (Project #3.py) to save information</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>Marriage after 14</t>
   </si>
@@ -43,147 +47,147 @@
   </si>
   <si>
     <t>Find marriage date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Compare marriage date to birth date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Remaining Stories</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Story Velocity</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Act Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Act Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Est Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Est Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Act Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Act Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Completed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Initials</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Last</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>First</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Email</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>LOC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Code Velocity</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Min</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Sprint</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Store birth date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Store death date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Compare birth and death dates</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Find marriage record for individual</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Review Results</t>
@@ -244,7 +248,7 @@
   </si>
   <si>
     <t>Hold a team meeting to plan for spint planning</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
@@ -335,19 +339,19 @@
   </si>
   <si>
     <t>Est Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Act Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Act Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Completed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Obtain GitHub account</t>
@@ -642,15 +646,15 @@
   </si>
   <si>
     <t>dc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>dc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>dcohron@stevens.edu</t>
@@ -744,47 +748,51 @@
   </si>
   <si>
     <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Est Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DNC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>jdoll@stevens.edu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>https://github.com/dcohron/AgileMethods/</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">   * Inputs in blue</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Set next meeting before end current meeting</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Encouraging team environment</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Double check each other for better of the team</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>dc, jd, aw</t>
@@ -808,9 +816,6 @@
     <t>Create a NOTE record at the beginning of the file and include AgileMethods, the GitHub respository</t>
   </si>
   <si>
-    <t>Modify program (insert program name) to save information</t>
-  </si>
-  <si>
     <t>T04.01</t>
   </si>
   <si>
@@ -883,9 +888,6 @@
     <t>T06.03</t>
   </si>
   <si>
-    <t xml:space="preserve"> Store birth date</t>
-  </si>
-  <si>
     <t>Find death date</t>
   </si>
   <si>
@@ -899,17 +901,37 @@
   </si>
   <si>
     <t>store children's birth dates</t>
+  </si>
+  <si>
+    <t>DNC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DNC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Store birth date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+  <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="m/d"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -990,54 +1012,61 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1125,25 +1154,25 @@
           </c:extLst>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="69867128"/>
-        <c:axId val="508016824"/>
+        <c:axId val="508541624"/>
+        <c:axId val="507736088"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="69867128"/>
+        <c:axId val="508541624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="508016824"/>
+        <c:crossAx val="507736088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="508016824"/>
+        <c:axId val="507736088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1151,7 +1180,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69867128"/>
+        <c:crossAx val="508541624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1202,10 +1231,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1217,25 +1246,25 @@
           </c:extLst>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="508187400"/>
-        <c:axId val="508190520"/>
+        <c:axId val="461806088"/>
+        <c:axId val="506686408"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="508187400"/>
+        <c:axId val="461806088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="508190520"/>
+        <c:crossAx val="506686408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="508190520"/>
+        <c:axId val="506686408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,7 +1272,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="508187400"/>
+        <c:crossAx val="461806088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2092,85 +2121,85 @@
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="D9" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
   </hyperlinks>
@@ -2188,7 +2217,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -2199,479 +2228,480 @@
   <sheetData>
     <row r="1" spans="1:3" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A3" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A4" s="21" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A5" s="21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A6" s="21" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A7" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A13" s="21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="21" customFormat="1" ht="15">
       <c r="A15" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="21" customFormat="1" ht="15">
       <c r="A17" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A23" s="21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B23" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A25" s="21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A26" s="21" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="21" customFormat="1">
       <c r="A27" s="21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A29" s="21" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A31" s="24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30">
       <c r="A32" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A33" s="21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A34" s="21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A35" s="21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A36" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="21" customFormat="1" ht="15">
       <c r="A37" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A38" s="21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A39" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A40" s="21" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A41" s="21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15">
       <c r="A42" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A43" s="21" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -2686,7 +2716,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -2700,19 +2730,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1"/>
@@ -2728,16 +2758,22 @@
         <f>Stories!B3</f>
         <v>Birth before marriage</v>
       </c>
+      <c r="D3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2758,10 +2794,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3025,7 +3061,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3055,60 +3091,60 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1">
       <c r="A14" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B15" s="17">
         <v>41065</v>
@@ -3124,7 +3160,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B16" s="17">
         <v>41078</v>
@@ -3149,7 +3185,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B17" s="17">
         <v>41092</v>
@@ -3174,7 +3210,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B18" s="17">
         <v>41106</v>
@@ -3199,7 +3235,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="11" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B19" s="17">
         <v>41120</v>
@@ -3223,7 +3259,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
@@ -3239,7 +3275,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -3254,22 +3290,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3277,7 +3313,7 @@
         <v>41426</v>
       </c>
       <c r="B2" s="2">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -3289,7 +3325,7 @@
         <v>41431</v>
       </c>
       <c r="B3" s="2">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <f>B2-B3</f>
@@ -3308,11 +3344,12 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
@@ -3327,8 +3364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -3346,54 +3383,54 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I2" s="11">
         <v>41426</v>
@@ -3401,27 +3438,27 @@
     </row>
     <row r="3" spans="1:9" ht="26">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="26">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I5" s="11">
         <v>41426</v>
@@ -3429,16 +3466,16 @@
     </row>
     <row r="6" spans="1:9" ht="26">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I6" s="11">
         <v>41426</v>
@@ -3446,13 +3483,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I8" s="11">
         <v>41426</v>
@@ -3460,16 +3497,16 @@
     </row>
     <row r="9" spans="1:9" ht="26">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I9" s="11">
         <v>41426</v>
@@ -3477,43 +3514,43 @@
     </row>
     <row r="10" spans="1:9" ht="52">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" t="s">
         <v>191</v>
-      </c>
-      <c r="D10" t="s">
-        <v>190</v>
       </c>
       <c r="I10" s="11">
         <v>41426</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="39">
+    <row r="12" spans="1:9" ht="26">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>240</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="52">
       <c r="A13" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="52">
       <c r="A14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3521,85 +3558,94 @@
     </row>
     <row r="16" spans="1:9" ht="26">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="39">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="39">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="39">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="39">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="52">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="52">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="52">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="52">
       <c r="A20" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="B21" s="20"/>
     </row>
-    <row r="22" spans="1:2" ht="26">
+    <row r="22" spans="1:9" ht="26">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="39">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="39">
       <c r="A23" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="B24" s="20"/>
     </row>
-    <row r="25" spans="1:2" ht="26">
+    <row r="25" spans="1:9" ht="26">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="26">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>235</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="11">
+        <v>41428</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="26">
       <c r="A26" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="2:2">
@@ -3607,18 +3653,19 @@
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3629,10 +3676,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -3649,31 +3696,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3696,22 +3743,27 @@
         <f>Backlog!C3</f>
         <v>Birth before marriage</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="C3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3" s="29"/>
       <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="23" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="C4" s="8"/>
+        <v>273</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
@@ -3721,12 +3773,11 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="23" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="C5" s="8"/>
+        <v>258</v>
+      </c>
       <c r="D5" s="8"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -3736,12 +3787,11 @@
     </row>
     <row r="6" spans="1:9" ht="26">
       <c r="A6" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>260</v>
-      </c>
-      <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -3752,7 +3802,6 @@
     <row r="7" spans="1:9">
       <c r="A7" s="23"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -3762,270 +3811,264 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>228</v>
       </c>
       <c r="E8">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="F8">
-        <v>60</v>
-      </c>
-      <c r="G8">
-        <v>120</v>
-      </c>
-      <c r="H8">
-        <v>90</v>
-      </c>
-      <c r="I8" s="10">
-        <v>40444</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>175</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="26" t="str">
+      <c r="A13" s="26" t="str">
         <f>Backlog!B5</f>
         <v>US04</v>
       </c>
-      <c r="B14" s="5" t="str">
+      <c r="B13" s="5" t="str">
         <f>Backlog!C5</f>
         <v>Marriage before divorce</v>
       </c>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>258</v>
+      </c>
       <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="23" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="26">
       <c r="A16" s="23" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="1:9" ht="26">
-      <c r="A17" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19">
+    <row r="18" spans="1:9">
+      <c r="A18" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18">
         <v>200</v>
       </c>
-      <c r="F19">
+      <c r="F18">
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="26">
+    <row r="20" spans="1:9" ht="26">
+      <c r="A20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="26">
       <c r="A22" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="26">
-      <c r="A23" t="s">
-        <v>178</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="26" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="26" t="str">
         <f>Backlog!B7</f>
         <v>US06</v>
       </c>
-      <c r="B25" s="5" t="str">
+      <c r="B24" s="5" t="str">
         <f>Backlog!C7</f>
         <v>Divorce before death</v>
       </c>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>259</v>
+      </c>
       <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="23" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" ht="26">
       <c r="A27" s="23" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" ht="26">
-      <c r="A28" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>267</v>
-      </c>
+    <row r="28" spans="1:9">
+      <c r="A28" s="23"/>
+      <c r="B28" s="25"/>
       <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="23"/>
-      <c r="B29" s="25"/>
-      <c r="I29" s="11"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="26" t="str">
+      <c r="A29" s="26" t="str">
         <f>Backlog!B8</f>
         <v>US12</v>
       </c>
-      <c r="B30" s="25" t="str">
+      <c r="B29" s="25" t="str">
         <f>Backlog!C8</f>
         <v>Parents not too old</v>
       </c>
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>268</v>
+      </c>
       <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="23" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" ht="26">
       <c r="A33" s="23" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>270</v>
+        <v>182</v>
       </c>
       <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" ht="26">
       <c r="A34" s="23" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="1:9" ht="26">
-      <c r="A35" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>182</v>
-      </c>
+    <row r="35" spans="1:9">
+      <c r="B35" s="25"/>
       <c r="I35" s="11"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="B36" s="25"/>
-      <c r="I36" s="11"/>
+      <c r="B36" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="B37" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="B37" s="9"/>
+      <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="B38" s="9"/>
-      <c r="I38" s="11"/>
+      <c r="B38" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="B39" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="B39" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="26">
       <c r="B40" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="26">
-      <c r="B41" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="B42" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="26">
+      <c r="B43" s="5" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="B43" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="26">
-      <c r="B44" s="5" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4047,35 +4090,36 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4097,35 +4141,36 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4147,35 +4192,36 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
Update to Team Report
</commit_message>
<xml_diff>
--- a/TeamNick_Jeremy_AmieReport.xlsx
+++ b/TeamNick_Jeremy_AmieReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="21360" windowHeight="14400" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-180" yWindow="-100" windowWidth="21360" windowHeight="14400" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,759 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="285">
   <si>
+    <t>All male members of a family should have the same last name</t>
+  </si>
+  <si>
+    <t>Parents should not marry any of their descendants</t>
+  </si>
+  <si>
+    <t>Siblings should not marry one another</t>
+  </si>
+  <si>
+    <t>First cousins should not marry one another</t>
+  </si>
+  <si>
+    <t>Aunts and uncles should not marry their nieces or nephews</t>
+  </si>
+  <si>
+    <t>Divorce before death</t>
+  </si>
+  <si>
+    <t>Less then 150 years old</t>
+  </si>
+  <si>
+    <t>Death should be less than 150 years after birth for dead people, and current date should be less than 150 years after birth for all living people</t>
+  </si>
+  <si>
+    <t>Birth before death of parents</t>
+  </si>
+  <si>
+    <t>Modify program (Project #3.py) to save information</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marriage after 14</t>
+  </si>
+  <si>
+    <t>No bigamy</t>
+  </si>
+  <si>
+    <t>Parents not too old</t>
+  </si>
+  <si>
+    <t>Find marriage date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compare marriage date to birth date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remaining Stories</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Velocity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Owner</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Size</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Owner</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Est Size</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Est Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Size</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Completed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Initials</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>First</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code Velocity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Owner</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprint</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Store birth date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Store death date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compare birth and death dates</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find marriage record for individual</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review Results</t>
+  </si>
+  <si>
+    <t>Keep doing:</t>
+  </si>
+  <si>
+    <t>Avoid:</t>
+  </si>
+  <si>
+    <t>GitHub Username</t>
+  </si>
+  <si>
+    <t>GitHub Repository:</t>
+  </si>
+  <si>
+    <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
+  </si>
+  <si>
+    <t>Birth should occur before marriage of an individual</t>
+  </si>
+  <si>
+    <t>Birth should occur before death of an individual</t>
+  </si>
+  <si>
+    <t>Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
+  </si>
+  <si>
+    <t>Marriage should occur before death of either spouse</t>
+  </si>
+  <si>
+    <t>Divorce can only occur before death of both spouses</t>
+  </si>
+  <si>
+    <t>Marriage should not occur during marriage to another spouse</t>
+  </si>
+  <si>
+    <t>No more than five siblings should be born at the same time</t>
+  </si>
+  <si>
+    <t>There should be fewer than 15 siblings in a family</t>
+  </si>
+  <si>
+    <t>US25</t>
+  </si>
+  <si>
+    <t>US26</t>
+  </si>
+  <si>
+    <t>US27</t>
+  </si>
+  <si>
+    <t>US28</t>
+  </si>
+  <si>
+    <t>US29</t>
+  </si>
+  <si>
+    <t>US30</t>
+  </si>
+  <si>
+    <t>US31</t>
+  </si>
+  <si>
+    <t>US32</t>
+  </si>
+  <si>
+    <t>US33</t>
+  </si>
+  <si>
+    <t>US34</t>
+  </si>
+  <si>
+    <t>US35</t>
+  </si>
+  <si>
+    <t>US36</t>
+  </si>
+  <si>
+    <t>US37</t>
+  </si>
+  <si>
+    <t>US38</t>
+  </si>
+  <si>
+    <t>US39</t>
+  </si>
+  <si>
+    <t>US40</t>
+  </si>
+  <si>
+    <t>US41</t>
+  </si>
+  <si>
+    <t>US42</t>
+  </si>
+  <si>
+    <t>T03.01</t>
+  </si>
+  <si>
+    <t>T03.02</t>
+  </si>
+  <si>
+    <t>T03.03</t>
+  </si>
+  <si>
+    <t>T05.01</t>
+  </si>
+  <si>
+    <t>T05.02</t>
+  </si>
+  <si>
+    <t>Hold a team meeting to plan for spint planning</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
+  </si>
+  <si>
+    <t>No more than one individual with the same name and birth date should appear in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>No more than one child with the same name and birth date should appear in a family</t>
+  </si>
+  <si>
+    <t>Include person's current age when listing individuals</t>
+  </si>
+  <si>
+    <t>List all deceased individuals in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all living married people in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all living people over 30 who have never been married in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all multiple births in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all orphaned children (both parents dead and child &lt; 18 years old) in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all couples who were married when the older spouse was more than twice as old as the younger spouse</t>
+  </si>
+  <si>
+    <t>List all people in a GEDCOM file who were born in the last 30 days</t>
+  </si>
+  <si>
+    <t>List all people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t>List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t>List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
+  </si>
+  <si>
+    <t>List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
+  </si>
+  <si>
+    <t>Accept and use dates without days or without days and months</t>
+  </si>
+  <si>
+    <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
+    <t>Story Name</t>
+  </si>
+  <si>
+    <t>Story Description</t>
+  </si>
+  <si>
+    <t>Birth before death</t>
+  </si>
+  <si>
+    <t>Birth before marriage</t>
+  </si>
+  <si>
+    <t>Marriage before divorce</t>
+  </si>
+  <si>
+    <t>Marriage before death</t>
+  </si>
+  <si>
+    <t>List siblings in families by decreasing age, i.e. oldest siblings first</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Cohron</t>
+  </si>
+  <si>
+    <t>dcohron</t>
+  </si>
+  <si>
+    <t>jd</t>
+  </si>
+  <si>
+    <t>Jeremy</t>
+  </si>
+  <si>
+    <t>Doll</t>
+  </si>
+  <si>
+    <t>jeremydoll</t>
+  </si>
+  <si>
+    <t>Amie</t>
+  </si>
+  <si>
+    <t>Widerkehr</t>
+  </si>
+  <si>
+    <t>alwider</t>
+  </si>
+  <si>
+    <t>Story ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Child should be born before death of mother and before 9 months after death of father</t>
+  </si>
+  <si>
+    <t>Est Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Size</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Completed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Obtain GitHub account</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>T01.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each team member needs to obtain an account in GitHub </t>
+  </si>
+  <si>
+    <t>Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
+  </si>
+  <si>
+    <t>Siblings spacing</t>
+  </si>
+  <si>
+    <t>Fewer than 15 siblings</t>
+  </si>
+  <si>
+    <t>Male last names</t>
+  </si>
+  <si>
+    <t>No marriages to descendants</t>
+  </si>
+  <si>
+    <t>Siblings should not marry</t>
+  </si>
+  <si>
+    <t>First cousins should not marry</t>
+  </si>
+  <si>
+    <t>Aunts and uncles</t>
+  </si>
+  <si>
+    <t>Correct gender for role</t>
+  </si>
+  <si>
+    <t>Husband in family should be male and wife in family should be female</t>
+  </si>
+  <si>
+    <t>All individual IDs should be unique and all family IDs should be unique</t>
+  </si>
+  <si>
+    <t>Unique IDs</t>
+  </si>
+  <si>
+    <t>Unique name and birth date</t>
+  </si>
+  <si>
+    <t>Unique families by spouses</t>
+  </si>
+  <si>
+    <t>Unique first names in families</t>
+  </si>
+  <si>
+    <t>Corresponding entries</t>
+  </si>
+  <si>
+    <t>Include individual ages</t>
+  </si>
+  <si>
+    <t>Order siblings by age</t>
+  </si>
+  <si>
+    <t>List deceased</t>
+  </si>
+  <si>
+    <t>List living married</t>
+  </si>
+  <si>
+    <t>List living single</t>
+  </si>
+  <si>
+    <t>List multiple births</t>
+  </si>
+  <si>
+    <t>List orphans</t>
+  </si>
+  <si>
+    <t>List recent births</t>
+  </si>
+  <si>
+    <t>List recent deaths</t>
+  </si>
+  <si>
+    <t>List recent survivors</t>
+  </si>
+  <si>
+    <t>List upcoming birthdays</t>
+  </si>
+  <si>
+    <t>List upcoming anniversaries</t>
+  </si>
+  <si>
+    <t>Include input line numbers</t>
+  </si>
+  <si>
+    <t>List line numbers from GEDCOM source file when reporting errors</t>
+  </si>
+  <si>
+    <t>Include partial dates</t>
+  </si>
+  <si>
+    <t>Reject illegitimate dates</t>
+  </si>
+  <si>
+    <t>List large age differences</t>
+  </si>
+  <si>
+    <t>Story ID</t>
+  </si>
+  <si>
+    <t>US01</t>
+  </si>
+  <si>
+    <t>US02</t>
+  </si>
+  <si>
+    <t>US03</t>
+  </si>
+  <si>
+    <t>US04</t>
+  </si>
+  <si>
+    <t>US05</t>
+  </si>
+  <si>
+    <t>US06</t>
+  </si>
+  <si>
+    <t>US07</t>
+  </si>
+  <si>
+    <t>US08</t>
+  </si>
+  <si>
+    <t>US09</t>
+  </si>
+  <si>
+    <t>US10</t>
+  </si>
+  <si>
+    <t>US11</t>
+  </si>
+  <si>
+    <t>US12</t>
+  </si>
+  <si>
+    <t>US13</t>
+  </si>
+  <si>
+    <t>US14</t>
+  </si>
+  <si>
+    <t>US15</t>
+  </si>
+  <si>
+    <t>US16</t>
+  </si>
+  <si>
+    <t>US17</t>
+  </si>
+  <si>
+    <t>US18</t>
+  </si>
+  <si>
+    <t>US19</t>
+  </si>
+  <si>
+    <t>US20</t>
+  </si>
+  <si>
+    <t>US21</t>
+  </si>
+  <si>
+    <t>US22</t>
+  </si>
+  <si>
+    <t>US23</t>
+  </si>
+  <si>
+    <t>US24</t>
+  </si>
+  <si>
+    <t>Compare divorce date to death date</t>
+  </si>
+  <si>
+    <t>store mothers birth date</t>
+  </si>
+  <si>
+    <t>store fathers birth date</t>
+  </si>
+  <si>
+    <t>store children's birth dates</t>
+  </si>
+  <si>
+    <t>DNC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DNC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Store birth date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALW</t>
+  </si>
+  <si>
+    <t>DNC</t>
+  </si>
+  <si>
     <t>JRD</t>
+  </si>
+  <si>
+    <t>T05.03</t>
+  </si>
+  <si>
+    <t>Dates before current date</t>
+  </si>
+  <si>
+    <t>Birth before marriage of parents</t>
+  </si>
+  <si>
+    <t>Compare if mother is &lt; 60 years older than children</t>
+  </si>
+  <si>
+    <t>Compare if father is &lt; 80 years older than children</t>
+  </si>
+  <si>
+    <t>T12.01</t>
+  </si>
+  <si>
+    <t>T12.02</t>
+  </si>
+  <si>
+    <t>T12.03</t>
+  </si>
+  <si>
+    <t>T12.04</t>
+  </si>
+  <si>
+    <t>T12.05</t>
+  </si>
+  <si>
+    <t>alwider@sandia.gov</t>
+  </si>
+  <si>
+    <t>dc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dcohron@stevens.edu</t>
+  </si>
+  <si>
+    <t>to deliver the product.  Burndown charts can be done daily, weekly, at the end of a sprint, or at whatever time interval makes sense.</t>
+  </si>
+  <si>
+    <t>We'll update our burndown chart for the GEDCOM project at the end of each sprint.</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>At the end of each sprint, you should update the number of remaining stories, the LOC written to implement the user stories</t>
+  </si>
+  <si>
+    <t>implemented in this sprint, and the minutes needed to write those lines of code.</t>
+  </si>
+  <si>
+    <t>Here's a sample burndown chart for a team of three:</t>
+  </si>
+  <si>
+    <t>Multiple births &lt;= 5</t>
+  </si>
+  <si>
+    <t>Children should be born after marriage of parents (and not more than 9 months after their divorce)</t>
+  </si>
+  <si>
+    <t>Marriage should be at least 14 years after birth of both spouses (parents must be at least 14 years old)</t>
+  </si>
+  <si>
+    <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
+  </si>
+  <si>
+    <t>All family roles (spouse, child) specified in an individual record should have corresponding entries in the corresponding family records. Likewise, all individual roles (spouse, child) specified in family records should have corresponding entries in the corresponding  individual's records.  I.e. the information in the individual and family records should be consistent.</t>
+  </si>
+  <si>
+    <t>JRD</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -200,769 +952,13 @@
   </si>
   <si>
     <t>Find death date</t>
-  </si>
-  <si>
-    <t>Compare divorce date to death date</t>
-  </si>
-  <si>
-    <t>store mothers birth date</t>
-  </si>
-  <si>
-    <t>store fathers birth date</t>
-  </si>
-  <si>
-    <t>store children's birth dates</t>
-  </si>
-  <si>
-    <t>DNC</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DNC</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Store birth date</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALW</t>
-  </si>
-  <si>
-    <t>DNC</t>
-  </si>
-  <si>
-    <t>JRD</t>
-  </si>
-  <si>
-    <t>T05.03</t>
-  </si>
-  <si>
-    <t>Dates before current date</t>
-  </si>
-  <si>
-    <t>Birth before marriage of parents</t>
-  </si>
-  <si>
-    <t>Compare if mother is &lt; 60 years older than children</t>
-  </si>
-  <si>
-    <t>Compare if father is &lt; 80 years older than children</t>
-  </si>
-  <si>
-    <t>T12.01</t>
-  </si>
-  <si>
-    <t>T12.02</t>
-  </si>
-  <si>
-    <t>T12.03</t>
-  </si>
-  <si>
-    <t>T12.04</t>
-  </si>
-  <si>
-    <t>T12.05</t>
-  </si>
-  <si>
-    <t>alwider@sandia.gov</t>
-  </si>
-  <si>
-    <t>dc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>dc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>dcohron@stevens.edu</t>
-  </si>
-  <si>
-    <t>to deliver the product.  Burndown charts can be done daily, weekly, at the end of a sprint, or at whatever time interval makes sense.</t>
-  </si>
-  <si>
-    <t>We'll update our burndown chart for the GEDCOM project at the end of each sprint.</t>
-  </si>
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>At the end of each sprint, you should update the number of remaining stories, the LOC written to implement the user stories</t>
-  </si>
-  <si>
-    <t>implemented in this sprint, and the minutes needed to write those lines of code.</t>
-  </si>
-  <si>
-    <t>Here's a sample burndown chart for a team of three:</t>
-  </si>
-  <si>
-    <t>Multiple births &lt;= 5</t>
-  </si>
-  <si>
-    <t>Children should be born after marriage of parents (and not more than 9 months after their divorce)</t>
-  </si>
-  <si>
-    <t>Marriage should be at least 14 years after birth of both spouses (parents must be at least 14 years old)</t>
-  </si>
-  <si>
-    <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
-  </si>
-  <si>
-    <t>All family roles (spouse, child) specified in an individual record should have corresponding entries in the corresponding family records. Likewise, all individual roles (spouse, child) specified in family records should have corresponding entries in the corresponding  individual's records.  I.e. the information in the individual and family records should be consistent.</t>
-  </si>
-  <si>
-    <t>List siblings in families by decreasing age, i.e. oldest siblings first</t>
-  </si>
-  <si>
-    <t>dc</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Cohron</t>
-  </si>
-  <si>
-    <t>dcohron</t>
-  </si>
-  <si>
-    <t>jd</t>
-  </si>
-  <si>
-    <t>Jeremy</t>
-  </si>
-  <si>
-    <t>Doll</t>
-  </si>
-  <si>
-    <t>jeremydoll</t>
-  </si>
-  <si>
-    <t>Amie</t>
-  </si>
-  <si>
-    <t>Widerkehr</t>
-  </si>
-  <si>
-    <t>alwider</t>
-  </si>
-  <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Child should be born before death of mother and before 9 months after death of father</t>
-  </si>
-  <si>
-    <t>Est Time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Size</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Completed</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Obtain GitHub account</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>T01.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Each team member needs to obtain an account in GitHub </t>
-  </si>
-  <si>
-    <t>Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
-  </si>
-  <si>
-    <t>Siblings spacing</t>
-  </si>
-  <si>
-    <t>Fewer than 15 siblings</t>
-  </si>
-  <si>
-    <t>Male last names</t>
-  </si>
-  <si>
-    <t>No marriages to descendants</t>
-  </si>
-  <si>
-    <t>Siblings should not marry</t>
-  </si>
-  <si>
-    <t>First cousins should not marry</t>
-  </si>
-  <si>
-    <t>Aunts and uncles</t>
-  </si>
-  <si>
-    <t>Correct gender for role</t>
-  </si>
-  <si>
-    <t>Husband in family should be male and wife in family should be female</t>
-  </si>
-  <si>
-    <t>All individual IDs should be unique and all family IDs should be unique</t>
-  </si>
-  <si>
-    <t>Unique IDs</t>
-  </si>
-  <si>
-    <t>Unique name and birth date</t>
-  </si>
-  <si>
-    <t>Unique families by spouses</t>
-  </si>
-  <si>
-    <t>Unique first names in families</t>
-  </si>
-  <si>
-    <t>Corresponding entries</t>
-  </si>
-  <si>
-    <t>Include individual ages</t>
-  </si>
-  <si>
-    <t>Order siblings by age</t>
-  </si>
-  <si>
-    <t>List deceased</t>
-  </si>
-  <si>
-    <t>List living married</t>
-  </si>
-  <si>
-    <t>List living single</t>
-  </si>
-  <si>
-    <t>List multiple births</t>
-  </si>
-  <si>
-    <t>List orphans</t>
-  </si>
-  <si>
-    <t>List recent births</t>
-  </si>
-  <si>
-    <t>List recent deaths</t>
-  </si>
-  <si>
-    <t>List recent survivors</t>
-  </si>
-  <si>
-    <t>List upcoming birthdays</t>
-  </si>
-  <si>
-    <t>List upcoming anniversaries</t>
-  </si>
-  <si>
-    <t>Include input line numbers</t>
-  </si>
-  <si>
-    <t>List line numbers from GEDCOM source file when reporting errors</t>
-  </si>
-  <si>
-    <t>Include partial dates</t>
-  </si>
-  <si>
-    <t>Reject illegitimate dates</t>
-  </si>
-  <si>
-    <t>List large age differences</t>
-  </si>
-  <si>
-    <t>Story ID</t>
-  </si>
-  <si>
-    <t>US01</t>
-  </si>
-  <si>
-    <t>US02</t>
-  </si>
-  <si>
-    <t>US03</t>
-  </si>
-  <si>
-    <t>US04</t>
-  </si>
-  <si>
-    <t>US05</t>
-  </si>
-  <si>
-    <t>US06</t>
-  </si>
-  <si>
-    <t>US07</t>
-  </si>
-  <si>
-    <t>US08</t>
-  </si>
-  <si>
-    <t>US09</t>
-  </si>
-  <si>
-    <t>US10</t>
-  </si>
-  <si>
-    <t>US11</t>
-  </si>
-  <si>
-    <t>US12</t>
-  </si>
-  <si>
-    <t>US13</t>
-  </si>
-  <si>
-    <t>US14</t>
-  </si>
-  <si>
-    <t>US15</t>
-  </si>
-  <si>
-    <t>US16</t>
-  </si>
-  <si>
-    <t>US17</t>
-  </si>
-  <si>
-    <t>US18</t>
-  </si>
-  <si>
-    <t>US19</t>
-  </si>
-  <si>
-    <t>US20</t>
-  </si>
-  <si>
-    <t>US21</t>
-  </si>
-  <si>
-    <t>US22</t>
-  </si>
-  <si>
-    <t>US23</t>
-  </si>
-  <si>
-    <t>US24</t>
-  </si>
-  <si>
-    <t>US25</t>
-  </si>
-  <si>
-    <t>US26</t>
-  </si>
-  <si>
-    <t>US27</t>
-  </si>
-  <si>
-    <t>US28</t>
-  </si>
-  <si>
-    <t>US29</t>
-  </si>
-  <si>
-    <t>US30</t>
-  </si>
-  <si>
-    <t>US31</t>
-  </si>
-  <si>
-    <t>US32</t>
-  </si>
-  <si>
-    <t>US33</t>
-  </si>
-  <si>
-    <t>US34</t>
-  </si>
-  <si>
-    <t>US35</t>
-  </si>
-  <si>
-    <t>US36</t>
-  </si>
-  <si>
-    <t>US37</t>
-  </si>
-  <si>
-    <t>US38</t>
-  </si>
-  <si>
-    <t>US39</t>
-  </si>
-  <si>
-    <t>US40</t>
-  </si>
-  <si>
-    <t>US41</t>
-  </si>
-  <si>
-    <t>US42</t>
-  </si>
-  <si>
-    <t>T03.01</t>
-  </si>
-  <si>
-    <t>T03.02</t>
-  </si>
-  <si>
-    <t>T03.03</t>
-  </si>
-  <si>
-    <t>T05.01</t>
-  </si>
-  <si>
-    <t>T05.02</t>
-  </si>
-  <si>
-    <t>Hold a team meeting to plan for spint planning</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
-  </si>
-  <si>
-    <t>No more than one individual with the same name and birth date should appear in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>No more than one child with the same name and birth date should appear in a family</t>
-  </si>
-  <si>
-    <t>Include person's current age when listing individuals</t>
-  </si>
-  <si>
-    <t>List all deceased individuals in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all living married people in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all living people over 30 who have never been married in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all multiple births in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all orphaned children (both parents dead and child &lt; 18 years old) in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all couples who were married when the older spouse was more than twice as old as the younger spouse</t>
-  </si>
-  <si>
-    <t>List all people in a GEDCOM file who were born in the last 30 days</t>
-  </si>
-  <si>
-    <t>List all people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t>List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t>List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
-  </si>
-  <si>
-    <t>List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
-  </si>
-  <si>
-    <t>Accept and use dates without days or without days and months</t>
-  </si>
-  <si>
-    <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
-  </si>
-  <si>
-    <t>Story Name</t>
-  </si>
-  <si>
-    <t>Story Description</t>
-  </si>
-  <si>
-    <t>Birth before death</t>
-  </si>
-  <si>
-    <t>Birth before marriage</t>
-  </si>
-  <si>
-    <t>Marriage before divorce</t>
-  </si>
-  <si>
-    <t>Marriage before death</t>
-  </si>
-  <si>
-    <t>Divorce before death</t>
-  </si>
-  <si>
-    <t>Less then 150 years old</t>
-  </si>
-  <si>
-    <t>Death should be less than 150 years after birth for dead people, and current date should be less than 150 years after birth for all living people</t>
-  </si>
-  <si>
-    <t>Birth before death of parents</t>
-  </si>
-  <si>
-    <t>Modify program (Project #3.py) to save information</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Marriage after 14</t>
-  </si>
-  <si>
-    <t>No bigamy</t>
-  </si>
-  <si>
-    <t>Parents not too old</t>
-  </si>
-  <si>
-    <t>Find marriage date</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compare marriage date to birth date</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remaining Stories</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Velocity</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Size</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Est Size</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Est Time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Size</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Completed</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Initials</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Last</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>First</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Email</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOC</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code Velocity</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Min</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprint</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Store birth date</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Store death date</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compare birth and death dates</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Find marriage record for individual</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Review Results</t>
-  </si>
-  <si>
-    <t>Keep doing:</t>
-  </si>
-  <si>
-    <t>Avoid:</t>
-  </si>
-  <si>
-    <t>GitHub Username</t>
-  </si>
-  <si>
-    <t>GitHub Repository:</t>
-  </si>
-  <si>
-    <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
-  </si>
-  <si>
-    <t>Birth should occur before marriage of an individual</t>
-  </si>
-  <si>
-    <t>Birth should occur before death of an individual</t>
-  </si>
-  <si>
-    <t>Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
-  </si>
-  <si>
-    <t>Marriage should occur before death of either spouse</t>
-  </si>
-  <si>
-    <t>Divorce can only occur before death of both spouses</t>
-  </si>
-  <si>
-    <t>Marriage should not occur during marriage to another spouse</t>
-  </si>
-  <si>
-    <t>No more than five siblings should be born at the same time</t>
-  </si>
-  <si>
-    <t>There should be fewer than 15 siblings in a family</t>
-  </si>
-  <si>
-    <t>All male members of a family should have the same last name</t>
-  </si>
-  <si>
-    <t>Parents should not marry any of their descendants</t>
-  </si>
-  <si>
-    <t>Siblings should not marry one another</t>
-  </si>
-  <si>
-    <t>First cousins should not marry one another</t>
-  </si>
-  <si>
-    <t>Aunts and uncles should not marry their nieces or nephews</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
@@ -1192,27 +1188,26 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="69712344"/>
-        <c:axId val="69715400"/>
+        <c:axId val="510328392"/>
+        <c:axId val="510328744"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="69712344"/>
+        <c:axId val="510328392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69715400"/>
+        <c:crossAx val="510328744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="69715400"/>
+        <c:axId val="510328744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1220,7 +1215,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69712344"/>
+        <c:crossAx val="510328392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1285,27 +1280,26 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="501860168"/>
-        <c:axId val="501863288"/>
+        <c:axId val="507106280"/>
+        <c:axId val="507096376"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="501860168"/>
+        <c:axId val="507106280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="501863288"/>
+        <c:crossAx val="507096376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="501863288"/>
+        <c:axId val="507096376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1307,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="501860168"/>
+        <c:crossAx val="507106280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1349,7 +1343,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1387,7 +1381,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1452,7 +1446,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1521,7 +1515,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1591,7 +1585,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1660,7 +1654,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1730,7 +1724,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2087,78 +2081,78 @@
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>251</v>
+        <v>34</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>253</v>
+        <v>36</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>252</v>
+        <v>35</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>254</v>
+        <v>37</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>269</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>201</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>75</v>
+        <v>217</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>248</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>71</v>
+        <v>213</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="D9" s="8" t="s">
-        <v>270</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2194,478 +2188,479 @@
   <sheetData>
     <row r="1" spans="1:3" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>216</v>
+        <v>105</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>217</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>204</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>271</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A3" s="21" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>219</v>
+        <v>108</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>272</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A4" s="21" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>273</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A5" s="21" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>220</v>
+        <v>109</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>274</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="21" customFormat="1" ht="15">
       <c r="A6" s="21" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>221</v>
+        <v>110</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>275</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="21" customFormat="1" ht="15">
       <c r="A7" s="21" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>222</v>
+        <v>5</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>276</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
+        <v>6</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>224</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>205</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>88</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>8</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
-        <v>227</v>
+        <v>10</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>89</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>11</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>277</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A13" s="21" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>229</v>
+        <v>12</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>90</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="21" customFormat="1" ht="15">
       <c r="A15" s="21" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>87</v>
+        <v>229</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>278</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>279</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="21" customFormat="1" ht="15">
       <c r="A17" s="21" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>280</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>281</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>282</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>283</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="B21" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>284</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A23" s="21" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A25" s="21" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>200</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A26" s="21" t="s">
-        <v>174</v>
+        <v>63</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>201</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="21" customFormat="1">
       <c r="A27" s="21" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>202</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A29" s="21" t="s">
-        <v>177</v>
+        <v>66</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>203</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A31" s="24" t="s">
-        <v>179</v>
+        <v>68</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>204</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>205</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="21" customFormat="1" ht="15.75">
       <c r="A33" s="21" t="s">
-        <v>181</v>
+        <v>70</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>206</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A34" s="21" t="s">
-        <v>182</v>
+        <v>71</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>207</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A35" s="21" t="s">
-        <v>183</v>
+        <v>72</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>208</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A36" s="24" t="s">
-        <v>184</v>
+        <v>73</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>209</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="21" customFormat="1" ht="15">
       <c r="A37" s="21" t="s">
-        <v>185</v>
+        <v>74</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>210</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A38" s="21" t="s">
-        <v>186</v>
+        <v>75</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A39" s="21" t="s">
-        <v>187</v>
+        <v>76</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>212</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A40" s="21" t="s">
-        <v>188</v>
+        <v>77</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>213</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A41" s="21" t="s">
-        <v>189</v>
+        <v>78</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15">
       <c r="A42" t="s">
-        <v>190</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>214</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="21" customFormat="1" ht="30">
       <c r="A43" s="21" t="s">
-        <v>191</v>
+        <v>80</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>215</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2695,19 +2690,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>261</v>
+        <v>44</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>258</v>
+        <v>41</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>250</v>
+        <v>33</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>259</v>
+        <v>42</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>260</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1"/>
@@ -2724,7 +2719,7 @@
         <v>Birth before marriage</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2732,13 +2727,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2754,7 +2749,7 @@
         <v>Marriage before divorce</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2762,13 +2757,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>221</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2784,7 +2779,7 @@
         <v>Divorce before death</v>
       </c>
       <c r="D7" t="s">
-        <v>0</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2800,7 +2795,7 @@
         <v>Parents not too old</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3038,6 +3033,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3068,60 +3064,60 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
-        <v>198</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="11" t="s">
-        <v>76</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="11" t="s">
-        <v>77</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="11" t="s">
-        <v>85</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="11" t="s">
-        <v>86</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1">
       <c r="A14" s="8" t="s">
-        <v>78</v>
+        <v>220</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>232</v>
+        <v>15</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>233</v>
+        <v>16</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>234</v>
+        <v>17</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>255</v>
+        <v>38</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>257</v>
+        <v>40</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>256</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>221</v>
       </c>
       <c r="B15" s="17">
         <v>41426</v>
@@ -3137,7 +3133,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>222</v>
       </c>
       <c r="B16" s="17">
         <v>41438</v>
@@ -3162,7 +3158,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="11" t="s">
-        <v>81</v>
+        <v>223</v>
       </c>
       <c r="B17" s="17">
         <v>41452</v>
@@ -3187,7 +3183,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="11" t="s">
-        <v>82</v>
+        <v>224</v>
       </c>
       <c r="B18" s="17">
         <v>41466</v>
@@ -3212,7 +3208,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="11" t="s">
-        <v>83</v>
+        <v>225</v>
       </c>
       <c r="B19" s="17">
         <v>41487</v>
@@ -3267,22 +3263,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="7" t="s">
-        <v>232</v>
+        <v>15</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>233</v>
+        <v>16</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>234</v>
+        <v>17</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>255</v>
+        <v>38</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>257</v>
+        <v>40</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>256</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3321,7 +3317,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -3360,54 +3356,54 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>10</v>
+        <v>244</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>11</v>
+        <v>245</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>12</v>
+        <v>246</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="G2" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="H2" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="I2" s="11">
         <v>41426</v>
@@ -3415,27 +3411,27 @@
     </row>
     <row r="3" spans="1:9" ht="26">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>253</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="26">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>254</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I5" s="11">
         <v>41426</v>
@@ -3443,16 +3439,16 @@
     </row>
     <row r="6" spans="1:9" ht="26">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>255</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>256</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I6" s="11">
         <v>41426</v>
@@ -3460,13 +3456,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>23</v>
+        <v>257</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>215</v>
       </c>
       <c r="I8" s="11">
         <v>41426</v>
@@ -3474,16 +3470,16 @@
     </row>
     <row r="9" spans="1:9" ht="26">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>81</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>214</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>215</v>
       </c>
       <c r="I9" s="11">
         <v>41426</v>
@@ -3491,16 +3487,16 @@
     </row>
     <row r="10" spans="1:9" ht="52">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>82</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>216</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>215</v>
       </c>
       <c r="I10" s="11">
         <v>41426</v>
@@ -3508,16 +3504,16 @@
     </row>
     <row r="12" spans="1:9" ht="26">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>226</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>236</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I12" s="11">
         <v>41429</v>
@@ -3525,16 +3521,16 @@
     </row>
     <row r="13" spans="1:9" ht="52">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>260</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>27</v>
+        <v>261</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>237</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I13" s="11">
         <v>41429</v>
@@ -3542,16 +3538,16 @@
     </row>
     <row r="14" spans="1:9" ht="52">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>262</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>29</v>
+        <v>263</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>237</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I14" s="11">
         <v>41429</v>
@@ -3562,16 +3558,16 @@
     </row>
     <row r="16" spans="1:9" ht="26">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>30</v>
+        <v>264</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>238</v>
       </c>
       <c r="D16" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I16" s="11">
         <v>41430</v>
@@ -3579,16 +3575,16 @@
     </row>
     <row r="17" spans="1:9" ht="39">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>84</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>31</v>
+        <v>265</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>239</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I17" s="11">
         <v>41430</v>
@@ -3596,16 +3592,16 @@
     </row>
     <row r="18" spans="1:9" ht="39">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>85</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>32</v>
+        <v>266</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>239</v>
       </c>
       <c r="D18" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I18" s="11">
         <v>41430</v>
@@ -3613,16 +3609,16 @@
     </row>
     <row r="19" spans="1:9" ht="52">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>203</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>33</v>
+        <v>267</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>240</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I19" s="11">
         <v>41430</v>
@@ -3630,16 +3626,16 @@
     </row>
     <row r="20" spans="1:9" ht="52">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>268</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>35</v>
+        <v>269</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>239</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I20" s="11">
         <v>41430</v>
@@ -3650,16 +3646,16 @@
     </row>
     <row r="22" spans="1:9" ht="26">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>36</v>
+        <v>270</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>241</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I22" s="11">
         <v>41431</v>
@@ -3667,16 +3663,16 @@
     </row>
     <row r="23" spans="1:9" ht="39">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>271</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>38</v>
+        <v>272</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>242</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I23" s="11">
         <v>41431</v>
@@ -3687,16 +3683,16 @@
     </row>
     <row r="25" spans="1:9" ht="26">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>197</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>253</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I25" s="11">
         <v>41428</v>
@@ -3704,16 +3700,16 @@
     </row>
     <row r="26" spans="1:9" ht="26">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>273</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>40</v>
+        <v>274</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>253</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I26" s="11">
         <v>41428</v>
@@ -3721,7 +3717,7 @@
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="9" t="s">
-        <v>266</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="2:2">
@@ -3729,38 +3725,38 @@
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="9" t="s">
-        <v>267</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="5" t="s">
-        <v>17</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="26">
       <c r="B37" s="5" t="s">
-        <v>18</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="5" t="s">
-        <v>9</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="26">
       <c r="B39" s="5" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="9" t="s">
-        <v>268</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3773,7 +3769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -3791,31 +3787,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>241</v>
+        <v>24</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>242</v>
+        <v>25</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>243</v>
+        <v>26</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>244</v>
+        <v>27</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>245</v>
+        <v>28</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>246</v>
+        <v>29</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>247</v>
+        <v>30</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>248</v>
+        <v>31</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>249</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3839,7 +3835,7 @@
         <v>Birth before marriage</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>247</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3">
@@ -3854,10 +3850,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="23" t="s">
-        <v>21</v>
+        <v>255</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>57</v>
+        <v>199</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="14"/>
@@ -3868,10 +3864,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="23" t="s">
-        <v>41</v>
+        <v>275</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>42</v>
+        <v>276</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="14"/>
@@ -3882,10 +3878,10 @@
     </row>
     <row r="6" spans="1:9" ht="26">
       <c r="A6" s="23" t="s">
-        <v>46</v>
+        <v>280</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="14"/>
@@ -3906,13 +3902,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="26" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>247</v>
       </c>
       <c r="E8">
         <v>20</v>
@@ -3923,26 +3919,26 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>81</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>262</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>82</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>263</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>83</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>264</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3958,7 +3954,7 @@
         <v>Marriage before divorce</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="E13">
         <v>20</v>
@@ -3970,40 +3966,40 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="23" t="s">
-        <v>26</v>
+        <v>260</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>42</v>
+        <v>276</v>
       </c>
       <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="23" t="s">
-        <v>28</v>
+        <v>262</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>43</v>
+        <v>277</v>
       </c>
       <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" ht="26">
       <c r="A16" s="23" t="s">
-        <v>47</v>
+        <v>281</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>44</v>
+        <v>278</v>
       </c>
       <c r="I16" s="11"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="26" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>221</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -4014,26 +4010,26 @@
     </row>
     <row r="19" spans="1:9" ht="26">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>84</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>265</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>196</v>
+        <v>85</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>230</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="26">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>203</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>231</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -4046,7 +4042,7 @@
         <v>Divorce before death</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>202</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -4058,28 +4054,28 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="23" t="s">
-        <v>37</v>
+        <v>271</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>43</v>
+        <v>277</v>
       </c>
       <c r="I24" s="11"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="23" t="s">
-        <v>48</v>
+        <v>282</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:9" ht="26">
       <c r="A26" s="23" t="s">
-        <v>49</v>
+        <v>283</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>51</v>
+        <v>193</v>
       </c>
       <c r="I26" s="11"/>
     </row>
@@ -4098,7 +4094,7 @@
         <v>Parents not too old</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>202</v>
       </c>
       <c r="E28">
         <v>20</v>
@@ -4110,46 +4106,46 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="23" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="I29" s="11"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="23" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>53</v>
+        <v>195</v>
       </c>
       <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="23" t="s">
-        <v>68</v>
+        <v>210</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
       <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:9" ht="26">
       <c r="A32" s="23" t="s">
-        <v>69</v>
+        <v>211</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="I32" s="11"/>
     </row>
     <row r="33" spans="1:9" ht="26">
       <c r="A33" s="23" t="s">
-        <v>70</v>
+        <v>212</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>65</v>
+        <v>207</v>
       </c>
       <c r="I33" s="11"/>
     </row>
@@ -4159,7 +4155,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="B35" s="9" t="s">
-        <v>266</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -4168,18 +4164,18 @@
     </row>
     <row r="37" spans="1:9">
       <c r="B37" s="9" t="s">
-        <v>267</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="B41" s="9" t="s">
-        <v>268</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4200,34 +4196,35 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>241</v>
+        <v>24</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>242</v>
+        <v>25</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>243</v>
+        <v>26</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>244</v>
+        <v>27</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>245</v>
+        <v>28</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>246</v>
+        <v>29</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>247</v>
+        <v>30</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>248</v>
+        <v>31</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>249</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4250,34 +4247,35 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>235</v>
+        <v>18</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>236</v>
+        <v>19</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>237</v>
+        <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>238</v>
+        <v>21</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>245</v>
+        <v>28</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>246</v>
+        <v>29</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>239</v>
+        <v>22</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>240</v>
+        <v>23</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>249</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4300,34 +4298,35 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>235</v>
+        <v>18</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>236</v>
+        <v>19</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>237</v>
+        <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>238</v>
+        <v>21</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>245</v>
+        <v>28</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>246</v>
+        <v>29</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>239</v>
+        <v>22</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>240</v>
+        <v>23</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>249</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
more sprint 1 and reorganizing
</commit_message>
<xml_diff>
--- a/TeamNick_Jeremy_AmieReport.xlsx
+++ b/TeamNick_Jeremy_AmieReport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="21360" windowHeight="14400" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="225" yWindow="225" windowWidth="21360" windowHeight="14400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
     <sheet name="Stories" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="290">
   <si>
     <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
   </si>
@@ -964,17 +964,23 @@
   </si>
   <si>
     <t>Sort the individual collections in order by their unique identifiers</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1027,6 +1033,11 @@
       <color indexed="48"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1062,7 +1073,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1114,6 +1125,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1137,12 +1152,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1150,22 +1175,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41426.0</c:v>
+                  <c:v>41426</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41438.0</c:v>
+                  <c:v>41438</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41452.0</c:v>
+                  <c:v>41452</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41466.0</c:v>
+                  <c:v>41466</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41487.0</c:v>
+                  <c:v>41487</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1177,67 +1202,84 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D8B4-4A59-B4A6-22A62B3A8A42}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="509839112"/>
-        <c:axId val="509842264"/>
+        <c:smooth val="0"/>
+        <c:axId val="42255872"/>
+        <c:axId val="42257408"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="509839112"/>
+        <c:axId val="42255872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="509842264"/>
+        <c:crossAx val="42257408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="509842264"/>
+        <c:axId val="42257408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="509839112"/>
+        <c:crossAx val="42255872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1247,12 +1289,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1263,10 +1315,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41431.0</c:v>
+                  <c:v>41431</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41438.0</c:v>
+                  <c:v>41438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1278,58 +1330,75 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A765-4833-A692-C31CA7692FD8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="509850360"/>
-        <c:axId val="509847896"/>
+        <c:smooth val="0"/>
+        <c:axId val="113416448"/>
+        <c:axId val="110755840"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="509850360"/>
+        <c:axId val="113416448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="509847896"/>
+        <c:crossAx val="110755840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="509847896"/>
+        <c:axId val="110755840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="509850360"/>
+        <c:crossAx val="113416448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1355,7 +1424,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1393,7 +1462,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1458,7 +1527,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1527,7 +1596,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1597,7 +1666,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1666,7 +1735,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1736,7 +1805,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2076,22 +2145,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" customWidth="1"/>
+    <col min="3" max="3" width="8.375" customWidth="1"/>
+    <col min="4" max="5" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1">
+    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
@@ -2108,7 +2177,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -2125,7 +2194,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -2142,7 +2211,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>211</v>
       </c>
@@ -2159,7 +2228,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>65</v>
       </c>
@@ -2185,20 +2254,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1">
+    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>74</v>
       </c>
@@ -2209,7 +2278,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -2220,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="21" customFormat="1" ht="15.75">
+    <row r="3" spans="1:3" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>181</v>
       </c>
@@ -2231,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="21" customFormat="1" ht="15.75">
+    <row r="4" spans="1:3" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>182</v>
       </c>
@@ -2242,7 +2311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="5" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>183</v>
       </c>
@@ -2253,7 +2322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="21" customFormat="1" ht="15">
+    <row r="6" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>184</v>
       </c>
@@ -2264,7 +2333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="21" customFormat="1" ht="15">
+    <row r="7" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>185</v>
       </c>
@@ -2275,7 +2344,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>186</v>
       </c>
@@ -2286,7 +2355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>187</v>
       </c>
@@ -2297,7 +2366,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>188</v>
       </c>
@@ -2308,7 +2377,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>189</v>
       </c>
@@ -2319,7 +2388,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>190</v>
       </c>
@@ -2330,7 +2399,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="13" spans="1:3" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>191</v>
       </c>
@@ -2341,7 +2410,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>192</v>
       </c>
@@ -2352,7 +2421,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="21" customFormat="1" ht="15">
+    <row r="15" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>193</v>
       </c>
@@ -2363,7 +2432,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>194</v>
       </c>
@@ -2374,7 +2443,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="21" customFormat="1" ht="15">
+    <row r="17" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>195</v>
       </c>
@@ -2385,7 +2454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>196</v>
       </c>
@@ -2396,7 +2465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>197</v>
       </c>
@@ -2407,7 +2476,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>198</v>
       </c>
@@ -2418,7 +2487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>199</v>
       </c>
@@ -2429,7 +2498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>200</v>
       </c>
@@ -2440,7 +2509,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="23" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>201</v>
       </c>
@@ -2451,7 +2520,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>202</v>
       </c>
@@ -2462,7 +2531,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="25" spans="1:3" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
         <v>203</v>
       </c>
@@ -2473,7 +2542,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="26" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>80</v>
       </c>
@@ -2484,7 +2553,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="21" customFormat="1">
+    <row r="27" spans="1:3" s="21" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>81</v>
       </c>
@@ -2495,7 +2564,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -2506,7 +2575,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="29" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>83</v>
       </c>
@@ -2517,7 +2586,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -2528,7 +2597,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="21" customFormat="1" ht="15.75">
+    <row r="31" spans="1:3" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
         <v>85</v>
       </c>
@@ -2539,7 +2608,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -2550,7 +2619,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="21" customFormat="1" ht="15.75">
+    <row r="33" spans="1:3" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
         <v>87</v>
       </c>
@@ -2561,7 +2630,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="34" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
         <v>88</v>
       </c>
@@ -2572,7 +2641,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="35" spans="1:3" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>89</v>
       </c>
@@ -2583,7 +2652,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="36" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
         <v>90</v>
       </c>
@@ -2594,7 +2663,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="21" customFormat="1" ht="15">
+    <row r="37" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>91</v>
       </c>
@@ -2605,7 +2674,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="38" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
         <v>92</v>
       </c>
@@ -2616,7 +2685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="39" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>93</v>
       </c>
@@ -2627,7 +2696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="40" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
         <v>94</v>
       </c>
@@ -2638,7 +2707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="41" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
         <v>95</v>
       </c>
@@ -2649,7 +2718,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -2660,7 +2729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="21" customFormat="1" ht="30">
+    <row r="43" spans="1:3" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>97</v>
       </c>
@@ -2672,7 +2741,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2684,23 +2752,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1">
+    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>56</v>
       </c>
@@ -2717,8 +2785,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1"/>
-    <row r="3" spans="1:5" s="8" customFormat="1">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>1</v>
       </c>
@@ -2733,8 +2801,11 @@
       <c r="D3" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="32" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2747,8 +2818,11 @@
       <c r="D4" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2764,7 +2838,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2778,7 +2852,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2793,8 +2867,11 @@
       <c r="D7" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2809,8 +2886,11 @@
       <c r="D8" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2823,7 +2903,7 @@
         <v>Multiple births &lt;= 5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2836,7 +2916,7 @@
         <v>Male last names</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2849,7 +2929,7 @@
         <v>Unique IDs</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2862,7 +2942,7 @@
         <v>Unique families by spouses</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2875,7 +2955,7 @@
         <v>Unique first names in families</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2888,7 +2968,7 @@
         <v>Corresponding entries</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2901,7 +2981,7 @@
         <v>Order siblings by age</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2914,7 +2994,7 @@
         <v>List living married</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2927,7 +3007,7 @@
         <v>List multiple births</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2940,7 +3020,7 @@
         <v>List orphans</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2953,7 +3033,7 @@
         <v>List large age differences</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2966,7 +3046,7 @@
         <v>List recent births</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
@@ -2979,7 +3059,7 @@
         <v>List recent deaths</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2992,7 +3072,7 @@
         <v>List recent survivors</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3005,7 +3085,7 @@
         <v>List upcoming birthdays</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3018,7 +3098,7 @@
         <v>List upcoming anniversaries</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3031,7 +3111,7 @@
         <v>Include input line numbers</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -3047,6 +3127,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3056,54 +3137,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="11"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="8" customFormat="1">
+    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>231</v>
       </c>
@@ -3126,7 +3207,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>232</v>
       </c>
@@ -3142,7 +3223,7 @@
       <c r="F15" s="18"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -3167,7 +3248,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>234</v>
       </c>
@@ -3192,7 +3273,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>235</v>
       </c>
@@ -3217,7 +3298,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>236</v>
       </c>
@@ -3255,24 +3336,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="6"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>27</v>
       </c>
@@ -3292,7 +3373,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>41431</v>
       </c>
@@ -3304,7 +3385,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>41438</v>
       </c>
@@ -3326,7 +3407,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>257</v>
       </c>
@@ -3344,27 +3425,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="23.875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.75" customWidth="1"/>
+    <col min="4" max="4" width="11.625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.375" customWidth="1"/>
+    <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>138</v>
       </c>
@@ -3393,7 +3474,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -3419,7 +3500,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="26">
+    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -3433,7 +3514,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26">
+    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -3447,7 +3528,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="26">
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>277</v>
       </c>
@@ -3464,7 +3545,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>182</v>
       </c>
@@ -3478,7 +3559,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="26">
+    <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -3495,7 +3576,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="52">
+    <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -3512,7 +3593,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="26">
+    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>183</v>
       </c>
@@ -3529,7 +3610,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="52">
+    <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3546,7 +3627,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="52">
+    <row r="14" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>284</v>
       </c>
@@ -3563,10 +3644,10 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="20"/>
     </row>
-    <row r="16" spans="1:9" ht="26">
+    <row r="16" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>184</v>
       </c>
@@ -3583,7 +3664,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="39">
+    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -3600,7 +3681,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="39">
+    <row r="18" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -3617,7 +3698,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="52">
+    <row r="19" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>214</v>
       </c>
@@ -3634,7 +3715,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="52">
+    <row r="20" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>177</v>
       </c>
@@ -3651,10 +3732,10 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" s="20"/>
     </row>
-    <row r="22" spans="1:9" ht="26">
+    <row r="22" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>185</v>
       </c>
@@ -3671,7 +3752,7 @@
         <v>41431</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="39">
+    <row r="23" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>180</v>
       </c>
@@ -3688,10 +3769,10 @@
         <v>41431</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" s="20"/>
     </row>
-    <row r="25" spans="1:9" ht="26">
+    <row r="25" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>186</v>
       </c>
@@ -3708,7 +3789,7 @@
         <v>41428</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="26">
+    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>243</v>
       </c>
@@ -3725,46 +3806,45 @@
         <v>41428</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="26">
+    <row r="37" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="26">
+    <row r="39" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="9" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3776,26 +3856,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="2" max="2" width="24.375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="8.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>36</v>
       </c>
@@ -3824,7 +3904,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="8"/>
@@ -3835,7 +3915,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="15"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="str">
         <f>Backlog!B3</f>
         <v>US02</v>
@@ -3866,7 +3946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>277</v>
       </c>
@@ -3880,7 +3960,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>245</v>
       </c>
@@ -3894,7 +3974,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="15"/>
     </row>
-    <row r="6" spans="1:9" ht="26">
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>250</v>
       </c>
@@ -3908,7 +3988,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="23"/>
       <c r="B7" s="25"/>
       <c r="D7" s="8"/>
@@ -3918,7 +3998,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>182</v>
       </c>
@@ -3947,7 +4027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -3956,7 +4036,7 @@
       </c>
       <c r="I9" s="30"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -3965,7 +4045,7 @@
       </c>
       <c r="I10" s="30"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -3974,10 +4054,10 @@
       </c>
       <c r="I11" s="30"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I12" s="30"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="str">
         <f>Backlog!B5</f>
         <v>US04</v>
@@ -3997,7 +4077,7 @@
       </c>
       <c r="I13" s="30"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>282</v>
       </c>
@@ -4006,7 +4086,7 @@
       </c>
       <c r="I14" s="30"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>284</v>
       </c>
@@ -4015,7 +4095,7 @@
       </c>
       <c r="I15" s="30"/>
     </row>
-    <row r="16" spans="1:9" ht="26">
+    <row r="16" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>251</v>
       </c>
@@ -4024,10 +4104,10 @@
       </c>
       <c r="I16" s="30"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I17" s="30"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
         <v>184</v>
       </c>
@@ -4045,7 +4125,7 @@
       </c>
       <c r="I18" s="30"/>
     </row>
-    <row r="19" spans="1:9" ht="26">
+    <row r="19" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -4054,7 +4134,7 @@
       </c>
       <c r="I19" s="30"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>102</v>
       </c>
@@ -4063,7 +4143,7 @@
       </c>
       <c r="I20" s="30"/>
     </row>
-    <row r="21" spans="1:9" ht="26">
+    <row r="21" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>214</v>
       </c>
@@ -4072,10 +4152,10 @@
       </c>
       <c r="I21" s="30"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I22" s="30"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="str">
         <f>Backlog!B7</f>
         <v>US06</v>
@@ -4087,15 +4167,26 @@
       <c r="C23" t="s">
         <v>213</v>
       </c>
+      <c r="D23" t="s">
+        <v>289</v>
+      </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="F23">
         <v>20</v>
       </c>
-      <c r="I23" s="30"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>30</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
         <v>180</v>
       </c>
@@ -4104,7 +4195,7 @@
       </c>
       <c r="I24" s="30"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
         <v>252</v>
       </c>
@@ -4113,7 +4204,7 @@
       </c>
       <c r="I25" s="30"/>
     </row>
-    <row r="26" spans="1:9" ht="26">
+    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
         <v>253</v>
       </c>
@@ -4122,12 +4213,12 @@
       </c>
       <c r="I26" s="30"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
       <c r="I27" s="30"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="str">
         <f>Backlog!B8</f>
         <v>US12</v>
@@ -4139,15 +4230,26 @@
       <c r="C28" t="s">
         <v>213</v>
       </c>
+      <c r="D28" t="s">
+        <v>289</v>
+      </c>
       <c r="E28">
         <v>20</v>
       </c>
       <c r="F28">
         <v>40</v>
       </c>
-      <c r="I28" s="30"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="G28">
+        <v>30</v>
+      </c>
+      <c r="H28">
+        <v>30</v>
+      </c>
+      <c r="I28" s="31" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
         <v>219</v>
       </c>
@@ -4156,7 +4258,7 @@
       </c>
       <c r="I29" s="30"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
         <v>220</v>
       </c>
@@ -4165,7 +4267,7 @@
       </c>
       <c r="I30" s="30"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
         <v>221</v>
       </c>
@@ -4174,7 +4276,7 @@
       </c>
       <c r="I31" s="30"/>
     </row>
-    <row r="32" spans="1:9" ht="26">
+    <row r="32" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>222</v>
       </c>
@@ -4183,7 +4285,7 @@
       </c>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" ht="26">
+    <row r="33" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
         <v>223</v>
       </c>
@@ -4192,31 +4294,30 @@
       </c>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="25"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B35" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B37" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B41" s="9" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4228,16 +4329,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>36</v>
       </c>
@@ -4267,7 +4368,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4279,16 +4379,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -4318,7 +4418,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4330,16 +4429,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -4369,7 +4468,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
US22 and 24 complete
US22 and 24 complete including test file and Team Report updated.
</commit_message>
<xml_diff>
--- a/TeamNick_Jeremy_AmieReport.xlsx
+++ b/TeamNick_Jeremy_AmieReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alwider\Desktop\GitHub\AgileMethods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickcohron/Stevens/Agile Methods/Project/AgileMethods/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="225" yWindow="225" windowWidth="21360" windowHeight="14400" activeTab="1"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="21360" windowHeight="14400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <sheet name="Sprint4" sheetId="9" r:id="rId9"/>
     <sheet name="Stories" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="316">
   <si>
     <t>UniqueFirst Names in Families</t>
   </si>
@@ -1005,7 +1008,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
@@ -1362,7 +1365,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1443,7 +1446,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1463,10 +1466,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.3112399999999998E-2"/>
-          <c:y val="5.5869000000000002E-2"/>
-          <c:w val="0.90188800000000002"/>
-          <c:h val="0.84119600000000005"/>
+          <c:x val="0.0931124"/>
+          <c:y val="0.055869"/>
+          <c:w val="0.901888"/>
+          <c:h val="0.841196"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1509,22 +1512,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41426</c:v>
+                  <c:v>41426.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41438</c:v>
+                  <c:v>41438.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41452</c:v>
+                  <c:v>41452.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41466</c:v>
+                  <c:v>41466.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41487</c:v>
+                  <c:v>41487.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1536,25 +1539,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F845-4DB0-BF4B-61C3F2B72AD9}"/>
             </c:ext>
@@ -1570,11 +1573,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="504176216"/>
-        <c:axId val="504163960"/>
+        <c:axId val="878368768"/>
+        <c:axId val="878609904"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="504176216"/>
+        <c:axId val="878368768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1608,14 +1611,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="504163960"/>
+        <c:crossAx val="878609904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="504163960"/>
+        <c:axId val="878609904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1660,7 +1663,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="504176216"/>
+        <c:crossAx val="878368768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7.5"/>
@@ -1703,7 +1706,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1723,10 +1726,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.4069599999999999E-2"/>
-          <c:y val="5.5869000000000002E-2"/>
-          <c:w val="0.92093000000000003"/>
-          <c:h val="0.84119600000000005"/>
+          <c:x val="0.0740696"/>
+          <c:y val="0.055869"/>
+          <c:w val="0.92093"/>
+          <c:h val="0.841196"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1772,13 +1775,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41431</c:v>
+                  <c:v>41431.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41446</c:v>
+                  <c:v>41446.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41459</c:v>
+                  <c:v>41459.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1790,16 +1793,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-60FF-4851-ABD9-FA91BB13A616}"/>
             </c:ext>
@@ -1815,11 +1818,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69831448"/>
-        <c:axId val="69829464"/>
+        <c:axId val="1001989552"/>
+        <c:axId val="1001992032"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="69831448"/>
+        <c:axId val="1001989552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1853,14 +1856,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69829464"/>
+        <c:crossAx val="1001992032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="69829464"/>
+        <c:axId val="1001992032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,11 +1908,11 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69831448"/>
+        <c:crossAx val="1001989552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="6"/>
-        <c:minorUnit val="3"/>
+        <c:majorUnit val="6.0"/>
+        <c:minorUnit val="3.0"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1967,7 +1970,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2003,7 +2006,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2022,7 +2025,7 @@
           <xdr:cNvPr id="3" name="Shape 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2125,7 +2128,7 @@
           <xdr:cNvPr id="4" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2147,7 +2150,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2226,7 +2229,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2245,7 +2248,7 @@
           <xdr:cNvPr id="6" name="Shape 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2348,7 +2351,7 @@
           <xdr:cNvPr id="7" name="Shape 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2370,7 +2373,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2449,7 +2452,7 @@
         <xdr:cNvPr id="11" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2468,7 +2471,7 @@
           <xdr:cNvPr id="9" name="Shape 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2571,7 +2574,7 @@
           <xdr:cNvPr id="10" name="Shape 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2593,7 +2596,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2719,7 +2722,7 @@
         <xdr:cNvPr id="14" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2738,7 +2741,7 @@
           <xdr:cNvPr id="12" name="Shape 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2841,7 +2844,7 @@
           <xdr:cNvPr id="13" name="Shape 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2863,7 +2866,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2942,7 +2945,7 @@
         <xdr:cNvPr id="17" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2961,7 +2964,7 @@
           <xdr:cNvPr id="15" name="Shape 15">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3064,7 +3067,7 @@
           <xdr:cNvPr id="16" name="Shape 16">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000010000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3086,7 +3089,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3170,7 +3173,7 @@
         <xdr:cNvPr id="19" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4296,20 +4299,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="20.375" style="1" customWidth="1"/>
-    <col min="6" max="256" width="11" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="20.33203125" style="1" customWidth="1"/>
+    <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>193</v>
       </c>
@@ -4326,14 +4329,14 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>198</v>
       </c>
@@ -4350,7 +4353,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>203</v>
       </c>
@@ -4367,7 +4370,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>208</v>
       </c>
@@ -4384,28 +4387,28 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4416,7 +4419,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4431,31 +4434,27 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="44" customWidth="1"/>
-    <col min="2" max="2" width="28.125" style="44" customWidth="1"/>
-    <col min="3" max="3" width="49.375" style="44" customWidth="1"/>
-    <col min="4" max="256" width="11" style="44" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" style="44" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" style="44" customWidth="1"/>
+    <col min="4" max="5" width="11" style="44" customWidth="1"/>
+    <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>216</v>
       </c>
@@ -4468,7 +4467,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>155</v>
       </c>
@@ -4481,7 +4480,7 @@
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="47" t="s">
         <v>220</v>
       </c>
@@ -4494,7 +4493,7 @@
       <c r="D3" s="50"/>
       <c r="E3" s="51"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="47" t="s">
         <v>223</v>
       </c>
@@ -4507,7 +4506,7 @@
       <c r="D4" s="50"/>
       <c r="E4" s="51"/>
     </row>
-    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="47" t="s">
         <v>238</v>
       </c>
@@ -4520,7 +4519,7 @@
       <c r="D5" s="50"/>
       <c r="E5" s="51"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="47" t="s">
         <v>240</v>
       </c>
@@ -4533,7 +4532,7 @@
       <c r="D6" s="50"/>
       <c r="E6" s="51"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="47" t="s">
         <v>242</v>
       </c>
@@ -4546,7 +4545,7 @@
       <c r="D7" s="50"/>
       <c r="E7" s="51"/>
     </row>
-    <row r="8" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="52" t="s">
         <v>185</v>
       </c>
@@ -4559,7 +4558,7 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
@@ -4572,7 +4571,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>163</v>
       </c>
@@ -4585,7 +4584,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>166</v>
       </c>
@@ -4598,7 +4597,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
         <v>169</v>
       </c>
@@ -4611,7 +4610,7 @@
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
     </row>
-    <row r="13" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="47" t="s">
         <v>245</v>
       </c>
@@ -4624,7 +4623,7 @@
       <c r="D13" s="50"/>
       <c r="E13" s="51"/>
     </row>
-    <row r="14" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="55" t="s">
         <v>64</v>
       </c>
@@ -4637,7 +4636,7 @@
       <c r="D14" s="57"/>
       <c r="E14" s="57"/>
     </row>
-    <row r="15" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="47" t="s">
         <v>247</v>
       </c>
@@ -4650,7 +4649,7 @@
       <c r="D15" s="50"/>
       <c r="E15" s="51"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="55" t="s">
         <v>68</v>
       </c>
@@ -4663,7 +4662,7 @@
       <c r="D16" s="57"/>
       <c r="E16" s="57"/>
     </row>
-    <row r="17" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="47" t="s">
         <v>250</v>
       </c>
@@ -4676,7 +4675,7 @@
       <c r="D17" s="50"/>
       <c r="E17" s="51"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="52" t="s">
         <v>72</v>
       </c>
@@ -4689,7 +4688,7 @@
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -4702,7 +4701,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>78</v>
       </c>
@@ -4715,7 +4714,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>81</v>
       </c>
@@ -4728,7 +4727,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
@@ -4741,7 +4740,7 @@
       <c r="D22" s="46"/>
       <c r="E22" s="46"/>
     </row>
-    <row r="23" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="47" t="s">
         <v>252</v>
       </c>
@@ -4754,7 +4753,7 @@
       <c r="D23" s="50"/>
       <c r="E23" s="51"/>
     </row>
-    <row r="24" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="55" t="s">
         <v>25</v>
       </c>
@@ -4767,7 +4766,7 @@
       <c r="D24" s="57"/>
       <c r="E24" s="57"/>
     </row>
-    <row r="25" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="47" t="s">
         <v>254</v>
       </c>
@@ -4780,7 +4779,7 @@
       <c r="D25" s="50"/>
       <c r="E25" s="51"/>
     </row>
-    <row r="26" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="47" t="s">
         <v>256</v>
       </c>
@@ -4793,7 +4792,7 @@
       <c r="D26" s="50"/>
       <c r="E26" s="51"/>
     </row>
-    <row r="27" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="47" t="s">
         <v>258</v>
       </c>
@@ -4806,7 +4805,7 @@
       <c r="D27" s="50"/>
       <c r="E27" s="51"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="55" t="s">
         <v>108</v>
       </c>
@@ -4819,7 +4818,7 @@
       <c r="D28" s="57"/>
       <c r="E28" s="57"/>
     </row>
-    <row r="29" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="47" t="s">
         <v>260</v>
       </c>
@@ -4832,7 +4831,7 @@
       <c r="D29" s="50"/>
       <c r="E29" s="51"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="55" t="s">
         <v>33</v>
       </c>
@@ -4845,7 +4844,7 @@
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="47" t="s">
         <v>262</v>
       </c>
@@ -4858,7 +4857,7 @@
       <c r="D31" s="50"/>
       <c r="E31" s="51"/>
     </row>
-    <row r="32" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="55" t="s">
         <v>37</v>
       </c>
@@ -4871,7 +4870,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="47" t="s">
         <v>264</v>
       </c>
@@ -4884,7 +4883,7 @@
       <c r="D33" s="50"/>
       <c r="E33" s="51"/>
     </row>
-    <row r="34" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="47" t="s">
         <v>266</v>
       </c>
@@ -4897,7 +4896,7 @@
       <c r="D34" s="50"/>
       <c r="E34" s="51"/>
     </row>
-    <row r="35" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="47" t="s">
         <v>268</v>
       </c>
@@ -4910,7 +4909,7 @@
       <c r="D35" s="50"/>
       <c r="E35" s="51"/>
     </row>
-    <row r="36" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="47" t="s">
         <v>270</v>
       </c>
@@ -4923,7 +4922,7 @@
       <c r="D36" s="50"/>
       <c r="E36" s="51"/>
     </row>
-    <row r="37" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="47" t="s">
         <v>272</v>
       </c>
@@ -4936,7 +4935,7 @@
       <c r="D37" s="50"/>
       <c r="E37" s="51"/>
     </row>
-    <row r="38" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="47" t="s">
         <v>274</v>
       </c>
@@ -4949,7 +4948,7 @@
       <c r="D38" s="50"/>
       <c r="E38" s="51"/>
     </row>
-    <row r="39" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="47" t="s">
         <v>276</v>
       </c>
@@ -4962,7 +4961,7 @@
       <c r="D39" s="50"/>
       <c r="E39" s="51"/>
     </row>
-    <row r="40" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="47" t="s">
         <v>278</v>
       </c>
@@ -4975,7 +4974,7 @@
       <c r="D40" s="50"/>
       <c r="E40" s="51"/>
     </row>
-    <row r="41" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="47" t="s">
         <v>280</v>
       </c>
@@ -4988,7 +4987,7 @@
       <c r="D41" s="50"/>
       <c r="E41" s="51"/>
     </row>
-    <row r="42" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="55" t="s">
         <v>57</v>
       </c>
@@ -5001,7 +5000,7 @@
       <c r="D42" s="57"/>
       <c r="E42" s="57"/>
     </row>
-    <row r="43" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="58" t="s">
         <v>282</v>
       </c>
@@ -5020,33 +5019,28 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.375" style="5" customWidth="1"/>
-    <col min="6" max="256" width="11" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="5" customWidth="1"/>
+    <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>215</v>
       </c>
@@ -5063,14 +5057,14 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -5089,7 +5083,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -5106,7 +5100,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -5125,7 +5119,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -5142,7 +5136,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -5161,7 +5155,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -5180,14 +5174,14 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>2</v>
       </c>
@@ -5206,7 +5200,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>2</v>
       </c>
@@ -5225,7 +5219,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6">
         <v>2</v>
       </c>
@@ -5241,10 +5235,10 @@
         <v>198</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6">
         <v>2</v>
       </c>
@@ -5260,10 +5254,10 @@
         <v>198</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6">
         <v>2</v>
       </c>
@@ -5282,7 +5276,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6">
         <v>2</v>
       </c>
@@ -5301,14 +5295,14 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6">
         <v>3</v>
       </c>
@@ -5327,7 +5321,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="6">
         <v>3</v>
       </c>
@@ -5346,7 +5340,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6">
         <v>3</v>
       </c>
@@ -5361,7 +5355,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6">
         <v>3</v>
       </c>
@@ -5376,7 +5370,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6">
         <v>3</v>
       </c>
@@ -5388,10 +5382,14 @@
         <f>Stories!B35</f>
         <v>List large age differences</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6">
         <v>3</v>
       </c>
@@ -5403,17 +5401,21 @@
         <f>Stories!B36</f>
         <v>List recent births</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="6">
         <v>4</v>
       </c>
@@ -5428,7 +5430,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6">
         <v>4</v>
       </c>
@@ -5443,7 +5445,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="6">
         <v>4</v>
       </c>
@@ -5458,7 +5460,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="6">
         <v>4</v>
       </c>
@@ -5473,7 +5475,7 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="6">
         <v>4</v>
       </c>
@@ -5488,7 +5490,7 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="6">
         <v>4</v>
       </c>
@@ -5509,32 +5511,28 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="15.875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="6.875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="8" customWidth="1"/>
-    <col min="7" max="256" width="11" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="8" customWidth="1"/>
+    <col min="7" max="8" width="11" style="8" customWidth="1"/>
+    <col min="9" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>284</v>
       </c>
@@ -5546,7 +5544,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>285</v>
       </c>
@@ -5558,7 +5556,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>286</v>
       </c>
@@ -5570,7 +5568,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -5580,7 +5578,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>287</v>
       </c>
@@ -5592,7 +5590,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
         <v>288</v>
       </c>
@@ -5604,7 +5602,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -5614,7 +5612,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>137</v>
       </c>
@@ -5626,7 +5624,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -5636,7 +5634,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5646,7 +5644,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -5656,7 +5654,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5666,7 +5664,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -5676,7 +5674,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>215</v>
       </c>
@@ -5700,7 +5698,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>144</v>
       </c>
@@ -5718,7 +5716,7 @@
       <c r="G15" s="17"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>145</v>
       </c>
@@ -5744,7 +5742,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
         <v>146</v>
       </c>
@@ -5770,7 +5768,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
         <v>147</v>
       </c>
@@ -5796,7 +5794,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
         <v>148</v>
       </c>
@@ -5822,7 +5820,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="3"/>
       <c r="C20" s="20"/>
@@ -5832,7 +5830,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -5842,7 +5840,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5852,7 +5850,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5862,7 +5860,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5872,7 +5870,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5882,7 +5880,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5892,7 +5890,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5902,7 +5900,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5912,7 +5910,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5922,7 +5920,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5932,7 +5930,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5942,7 +5940,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5952,7 +5950,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="10"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5962,7 +5960,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5972,7 +5970,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5982,7 +5980,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="10"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5992,7 +5990,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="10"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6002,7 +6000,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="10"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6012,7 +6010,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="10"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -6029,34 +6027,30 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="22" customWidth="1"/>
-    <col min="2" max="2" width="16.625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="12.375" style="22" customWidth="1"/>
-    <col min="4" max="4" width="7.125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="22" customWidth="1"/>
-    <col min="7" max="256" width="11" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="11" style="22" customWidth="1"/>
+    <col min="8" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>138</v>
       </c>
@@ -6077,7 +6071,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="23">
         <v>41431</v>
       </c>
@@ -6092,7 +6086,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="23">
         <v>41446</v>
       </c>
@@ -6117,7 +6111,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>41459</v>
       </c>
@@ -6128,7 +6122,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6137,7 +6131,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6146,7 +6140,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6155,7 +6149,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="27" t="s">
         <v>149</v>
       </c>
@@ -6166,7 +6160,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -6175,7 +6169,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -6184,7 +6178,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -6193,7 +6187,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6202,7 +6196,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6211,7 +6205,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -6220,7 +6214,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -6229,7 +6223,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6238,7 +6232,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -6247,7 +6241,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6256,7 +6250,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6265,7 +6259,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6274,7 +6268,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6283,7 +6277,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6292,7 +6286,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6301,7 +6295,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6310,7 +6304,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6319,7 +6313,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6335,34 +6329,30 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="23.875" style="28" customWidth="1"/>
-    <col min="3" max="3" width="12.875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="11.625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="28" customWidth="1"/>
     <col min="5" max="5" width="12" style="28" customWidth="1"/>
-    <col min="6" max="6" width="11.375" style="28" customWidth="1"/>
-    <col min="7" max="7" width="8.375" style="28" customWidth="1"/>
-    <col min="8" max="8" width="9.375" style="28" customWidth="1"/>
-    <col min="9" max="256" width="11" style="28" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="28" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="28" customWidth="1"/>
+    <col min="9" max="9" width="11" style="28" customWidth="1"/>
+    <col min="10" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -6391,7 +6381,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>155</v>
       </c>
@@ -6418,7 +6408,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>159</v>
       </c>
@@ -6437,7 +6427,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" s="33"/>
       <c r="C4" s="3"/>
@@ -6448,7 +6438,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>220</v>
       </c>
@@ -6467,7 +6457,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>290</v>
       </c>
@@ -6488,7 +6478,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="33"/>
       <c r="C7" s="3"/>
@@ -6499,7 +6489,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>223</v>
       </c>
@@ -6518,7 +6508,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>294</v>
       </c>
@@ -6539,7 +6529,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>296</v>
       </c>
@@ -6560,7 +6550,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="33"/>
       <c r="C11" s="3"/>
@@ -6571,7 +6561,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>238</v>
       </c>
@@ -6592,7 +6582,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>300</v>
       </c>
@@ -6613,7 +6603,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>302</v>
       </c>
@@ -6634,7 +6624,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="33"/>
       <c r="C15" s="3"/>
@@ -6645,7 +6635,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -6666,7 +6656,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>174</v>
       </c>
@@ -6687,7 +6677,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>176</v>
       </c>
@@ -6708,7 +6698,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>178</v>
       </c>
@@ -6729,7 +6719,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>180</v>
       </c>
@@ -6750,7 +6740,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="33"/>
       <c r="C21" s="3"/>
@@ -6761,7 +6751,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>242</v>
       </c>
@@ -6782,7 +6772,7 @@
         <v>41431</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>183</v>
       </c>
@@ -6803,7 +6793,7 @@
         <v>41431</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="33"/>
       <c r="C24" s="3"/>
@@ -6814,7 +6804,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>185</v>
       </c>
@@ -6835,7 +6825,7 @@
         <v>41428</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>187</v>
       </c>
@@ -6856,7 +6846,7 @@
         <v>41428</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="33"/>
       <c r="C27" s="3"/>
@@ -6867,7 +6857,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="33"/>
       <c r="C28" s="3"/>
@@ -6878,7 +6868,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="33"/>
       <c r="C29" s="3"/>
@@ -6889,7 +6879,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="33"/>
       <c r="C30" s="3"/>
@@ -6900,7 +6890,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="33"/>
       <c r="C31" s="3"/>
@@ -6911,7 +6901,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="33"/>
       <c r="C32" s="3"/>
@@ -6922,7 +6912,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="29" t="s">
         <v>189</v>
@@ -6935,7 +6925,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="29"/>
       <c r="C34" s="3"/>
@@ -6946,7 +6936,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="29" t="s">
         <v>190</v>
@@ -6959,7 +6949,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="7" t="s">
         <v>191</v>
@@ -6972,7 +6962,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7" t="s">
         <v>192</v>
@@ -6985,7 +6975,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="7" t="s">
         <v>86</v>
@@ -6998,7 +6988,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7" t="s">
         <v>87</v>
@@ -7011,7 +7001,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="33"/>
       <c r="C40" s="3"/>
@@ -7022,7 +7012,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="29" t="s">
         <v>88</v>
@@ -7041,11 +7031,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7057,20 +7042,20 @@
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="34" customWidth="1"/>
-    <col min="2" max="2" width="24.375" style="34" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="34" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="34" customWidth="1"/>
     <col min="4" max="4" width="11" style="34" customWidth="1"/>
-    <col min="5" max="5" width="8.375" style="34" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="34" customWidth="1"/>
     <col min="6" max="6" width="9" style="34" customWidth="1"/>
-    <col min="7" max="7" width="8.375" style="34" customWidth="1"/>
-    <col min="8" max="8" width="9.375" style="34" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="34" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="34" customWidth="1"/>
     <col min="9" max="256" width="11" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -7099,7 +7084,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="35"/>
       <c r="B2" s="29"/>
       <c r="C2" s="35"/>
@@ -7110,7 +7095,7 @@
       <c r="H2" s="36"/>
       <c r="I2" s="37"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="str">
         <f>Backlog!B3</f>
         <v>US02</v>
@@ -7141,7 +7126,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>290</v>
       </c>
@@ -7156,7 +7141,7 @@
       <c r="H4" s="36"/>
       <c r="I4" s="37"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>91</v>
       </c>
@@ -7171,7 +7156,7 @@
       <c r="H5" s="36"/>
       <c r="I5" s="37"/>
     </row>
-    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>93</v>
       </c>
@@ -7186,7 +7171,7 @@
       <c r="H6" s="36"/>
       <c r="I6" s="37"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="3"/>
@@ -7197,7 +7182,7 @@
       <c r="H7" s="36"/>
       <c r="I7" s="37"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>223</v>
       </c>
@@ -7226,7 +7211,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>294</v>
       </c>
@@ -7241,7 +7226,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="40"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>296</v>
       </c>
@@ -7256,7 +7241,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="40"/>
     </row>
-    <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>96</v>
       </c>
@@ -7271,7 +7256,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="40"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="33"/>
       <c r="C12" s="3"/>
@@ -7282,7 +7267,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="40"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="str">
         <f>Backlog!B5</f>
         <v>US04</v>
@@ -7313,7 +7298,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>300</v>
       </c>
@@ -7328,7 +7313,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="40"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>302</v>
       </c>
@@ -7343,7 +7328,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="40"/>
     </row>
-    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
@@ -7358,7 +7343,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="40"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="33"/>
       <c r="C17" s="3"/>
@@ -7369,7 +7354,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="40"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>240</v>
       </c>
@@ -7398,7 +7383,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>174</v>
       </c>
@@ -7413,7 +7398,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="40"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>176</v>
       </c>
@@ -7428,7 +7413,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="40"/>
     </row>
-    <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>178</v>
       </c>
@@ -7443,7 +7428,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="40"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="33"/>
       <c r="C22" s="3"/>
@@ -7454,7 +7439,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="40"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="str">
         <f>Backlog!B7</f>
         <v>US06</v>
@@ -7485,7 +7470,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>183</v>
       </c>
@@ -7500,7 +7485,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="40"/>
     </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>104</v>
       </c>
@@ -7515,7 +7500,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="40"/>
     </row>
-    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>106</v>
       </c>
@@ -7530,7 +7515,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="40"/>
     </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="3"/>
@@ -7541,7 +7526,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="40"/>
     </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="str">
         <f>Backlog!B8</f>
         <v>US12</v>
@@ -7572,7 +7557,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>225</v>
       </c>
@@ -7587,7 +7572,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="40"/>
     </row>
-    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>227</v>
       </c>
@@ -7602,7 +7587,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="40"/>
     </row>
-    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>229</v>
       </c>
@@ -7617,7 +7602,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="40"/>
     </row>
-    <row r="32" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>231</v>
       </c>
@@ -7632,7 +7617,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>233</v>
       </c>
@@ -7647,7 +7632,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="7"/>
       <c r="C34" s="3"/>
@@ -7658,7 +7643,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="29" t="s">
         <v>189</v>
@@ -7677,7 +7662,7 @@
       </c>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="29"/>
       <c r="C36" s="3"/>
@@ -7688,7 +7673,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="29" t="s">
         <v>190</v>
@@ -7701,7 +7686,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="7" t="s">
         <v>235</v>
@@ -7714,7 +7699,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7" t="s">
         <v>236</v>
@@ -7727,7 +7712,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="66" t="s">
         <v>17</v>
@@ -7987,7 +7972,7 @@
       <c r="IU40" s="44"/>
       <c r="IV40" s="44"/>
     </row>
-    <row r="41" spans="1:256" ht="59.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:256" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="33" t="s">
         <v>62</v>
@@ -8000,7 +7985,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="29" t="s">
         <v>88</v>
@@ -8013,7 +7998,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="1:256" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:256" ht="89.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="33" t="s">
         <v>111</v>
@@ -8026,7 +8011,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="1:256" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:256" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3"/>
       <c r="B44" s="33" t="s">
         <v>112</v>
@@ -8039,7 +8024,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="B45" s="33" t="s">
         <v>113</v>
@@ -8052,7 +8037,7 @@
       <c r="H45" s="3"/>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="B46" s="33" t="s">
         <v>61</v>
@@ -8312,7 +8297,7 @@
       <c r="IU46" s="44"/>
       <c r="IV46" s="44"/>
     </row>
-    <row r="47" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="33" t="s">
         <v>18</v>
@@ -8578,11 +8563,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8590,18 +8570,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="41" customWidth="1"/>
     <col min="2" max="2" width="18" style="41" customWidth="1"/>
     <col min="3" max="256" width="11" style="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -8630,7 +8610,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>247</v>
       </c>
@@ -8660,7 +8640,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>115</v>
       </c>
@@ -8677,7 +8657,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>117</v>
       </c>
@@ -8694,7 +8674,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>119</v>
       </c>
@@ -8711,7 +8691,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="33"/>
       <c r="C6" s="3"/>
@@ -8722,7 +8702,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>250</v>
       </c>
@@ -8752,7 +8732,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>121</v>
       </c>
@@ -8767,7 +8747,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>123</v>
       </c>
@@ -8782,7 +8762,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
@@ -8797,7 +8777,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="33"/>
       <c r="C11" s="3"/>
@@ -8808,7 +8788,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>252</v>
       </c>
@@ -8833,9 +8813,11 @@
       <c r="H12" s="3">
         <v>75</v>
       </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>127</v>
       </c>
@@ -8850,7 +8832,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>129</v>
       </c>
@@ -8865,7 +8847,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="67" t="s">
         <v>19</v>
       </c>
@@ -9127,7 +9109,7 @@
       <c r="IU15" s="44"/>
       <c r="IV15" s="44"/>
     </row>
-    <row r="16" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="33"/>
       <c r="C16" s="3"/>
@@ -9138,7 +9120,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>254</v>
       </c>
@@ -9157,11 +9139,17 @@
       <c r="F17" s="6">
         <v>60</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17" s="3">
+        <v>40</v>
+      </c>
+      <c r="H17" s="3">
+        <v>120</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="18" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>131</v>
       </c>
@@ -9176,7 +9164,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>132</v>
       </c>
@@ -9191,7 +9179,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="67" t="s">
         <v>20</v>
       </c>
@@ -9453,7 +9441,7 @@
       <c r="IU20" s="44"/>
       <c r="IV20" s="44"/>
     </row>
-    <row r="21" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="35"/>
       <c r="B21" s="33"/>
       <c r="C21" s="3"/>
@@ -9464,7 +9452,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>256</v>
       </c>
@@ -9734,7 +9722,7 @@
       <c r="IU22" s="44"/>
       <c r="IV22" s="44"/>
     </row>
-    <row r="23" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -9996,7 +9984,7 @@
       <c r="IU23" s="44"/>
       <c r="IV23" s="44"/>
     </row>
-    <row r="24" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -10258,7 +10246,7 @@
       <c r="IU24" s="44"/>
       <c r="IV24" s="44"/>
     </row>
-    <row r="25" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="67" t="s">
         <v>21</v>
       </c>
@@ -10520,7 +10508,7 @@
       <c r="IU25" s="44"/>
       <c r="IV25" s="44"/>
     </row>
-    <row r="26" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2"/>
       <c r="B26" s="64"/>
       <c r="C26" s="3"/>
@@ -10778,7 +10766,7 @@
       <c r="IU26" s="44"/>
       <c r="IV26" s="44"/>
     </row>
-    <row r="27" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>258</v>
       </c>
@@ -11048,7 +11036,7 @@
       <c r="IU27" s="44"/>
       <c r="IV27" s="44"/>
     </row>
-    <row r="28" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
@@ -11310,7 +11298,7 @@
       <c r="IU28" s="44"/>
       <c r="IV28" s="44"/>
     </row>
-    <row r="29" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -11572,7 +11560,7 @@
       <c r="IU29" s="44"/>
       <c r="IV29" s="44"/>
     </row>
-    <row r="30" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -11834,7 +11822,7 @@
       <c r="IU30" s="44"/>
       <c r="IV30" s="44"/>
     </row>
-    <row r="31" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -12096,7 +12084,7 @@
       <c r="IU31" s="44"/>
       <c r="IV31" s="44"/>
     </row>
-    <row r="32" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="67" t="s">
         <v>22</v>
       </c>
@@ -12358,7 +12346,7 @@
       <c r="IU32" s="44"/>
       <c r="IV32" s="44"/>
     </row>
-    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2"/>
       <c r="B33" s="64"/>
       <c r="C33" s="3"/>
@@ -12622,11 +12610,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12638,14 +12621,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="42" customWidth="1"/>
-    <col min="2" max="2" width="21.25" style="42" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="42" customWidth="1"/>
     <col min="3" max="256" width="11" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -12674,7 +12657,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="68" t="str">
         <f>Backlog!$B$17</f>
         <v>US28</v>
@@ -12699,7 +12682,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
         <v>305</v>
       </c>
@@ -12961,7 +12944,7 @@
       <c r="IU3" s="44"/>
       <c r="IV3" s="44"/>
     </row>
-    <row r="4" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
         <v>306</v>
       </c>
@@ -13223,7 +13206,7 @@
       <c r="IU4" s="44"/>
       <c r="IV4" s="44"/>
     </row>
-    <row r="5" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
         <v>310</v>
       </c>
@@ -13485,7 +13468,7 @@
       <c r="IU5" s="44"/>
       <c r="IV5" s="44"/>
     </row>
-    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="70"/>
       <c r="B6" s="70"/>
       <c r="C6" s="69"/>
@@ -13743,7 +13726,7 @@
       <c r="IU6" s="44"/>
       <c r="IV6" s="44"/>
     </row>
-    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="68" t="str">
         <f>Backlog!$B$18</f>
         <v>US30</v>
@@ -13768,7 +13751,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="69" t="s">
         <v>309</v>
       </c>
@@ -13783,7 +13766,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="69" t="s">
         <v>314</v>
       </c>
@@ -13798,7 +13781,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="69" t="s">
         <v>315</v>
       </c>
@@ -13813,7 +13796,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -13824,7 +13807,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -13835,7 +13818,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -13846,7 +13829,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -13864,26 +13847,22 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="256" width="11" style="43" customWidth="1"/>
+    <col min="1" max="9" width="11" style="43" customWidth="1"/>
+    <col min="10" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -13912,7 +13891,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -13923,7 +13902,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -13934,7 +13913,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -13945,7 +13924,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -13956,7 +13935,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -13967,7 +13946,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -13978,7 +13957,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -13989,7 +13968,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -14000,7 +13979,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -14017,10 +13996,5 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated tests and excel
</commit_message>
<xml_diff>
--- a/TeamNick_Jeremy_AmieReport.xlsx
+++ b/TeamNick_Jeremy_AmieReport.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickcohron/Stevens/Agile Methods/Project/AgileMethods/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="21360" windowHeight="14400" activeTab="1"/>
+    <workbookView xWindow="225" yWindow="465" windowWidth="21360" windowHeight="14400" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,11 +18,8 @@
     <sheet name="Sprint4" sheetId="9" r:id="rId9"/>
     <sheet name="Stories" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="316">
   <si>
     <t>UniqueFirst Names in Families</t>
   </si>
@@ -1466,10 +1458,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0931124"/>
-          <c:y val="0.055869"/>
-          <c:w val="0.901888"/>
-          <c:h val="0.841196"/>
+          <c:x val="9.3112399999999998E-2"/>
+          <c:y val="5.5869000000000002E-2"/>
+          <c:w val="0.90188800000000002"/>
+          <c:h val="0.84119600000000005"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1512,22 +1504,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41426.0</c:v>
+                  <c:v>41426</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41438.0</c:v>
+                  <c:v>41438</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41452.0</c:v>
+                  <c:v>41452</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41466.0</c:v>
+                  <c:v>41466</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41487.0</c:v>
+                  <c:v>41487</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1539,19 +1531,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1573,11 +1565,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="878368768"/>
-        <c:axId val="878609904"/>
+        <c:axId val="41079168"/>
+        <c:axId val="41081088"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="878368768"/>
+        <c:axId val="41079168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1611,14 +1603,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="878609904"/>
+        <c:crossAx val="41081088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="878609904"/>
+        <c:axId val="41081088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1663,7 +1655,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="878368768"/>
+        <c:crossAx val="41079168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7.5"/>
@@ -1726,10 +1718,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0740696"/>
-          <c:y val="0.055869"/>
-          <c:w val="0.92093"/>
-          <c:h val="0.841196"/>
+          <c:x val="7.4069599999999999E-2"/>
+          <c:y val="5.5869000000000002E-2"/>
+          <c:w val="0.92093000000000003"/>
+          <c:h val="0.84119600000000005"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1775,13 +1767,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41431.0</c:v>
+                  <c:v>41431</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41446.0</c:v>
+                  <c:v>41446</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41459.0</c:v>
+                  <c:v>41459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1793,10 +1785,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1818,11 +1810,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1001989552"/>
-        <c:axId val="1001992032"/>
+        <c:axId val="101964032"/>
+        <c:axId val="101986688"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1001989552"/>
+        <c:axId val="101964032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1856,14 +1848,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1001992032"/>
+        <c:crossAx val="101986688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1001992032"/>
+        <c:axId val="101986688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1908,11 +1900,11 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1001989552"/>
+        <c:crossAx val="101964032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="6.0"/>
-        <c:minorUnit val="3.0"/>
+        <c:majorUnit val="6"/>
+        <c:minorUnit val="3"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1970,7 +1962,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2006,7 +1998,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2025,7 +2017,7 @@
           <xdr:cNvPr id="3" name="Shape 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2128,7 +2120,7 @@
           <xdr:cNvPr id="4" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2150,7 +2142,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2229,7 +2221,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2248,7 +2240,7 @@
           <xdr:cNvPr id="6" name="Shape 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2351,7 +2343,7 @@
           <xdr:cNvPr id="7" name="Shape 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2373,7 +2365,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2452,7 +2444,7 @@
         <xdr:cNvPr id="11" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2471,7 +2463,7 @@
           <xdr:cNvPr id="9" name="Shape 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2574,7 +2566,7 @@
           <xdr:cNvPr id="10" name="Shape 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2596,7 +2588,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2722,7 +2714,7 @@
         <xdr:cNvPr id="14" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2741,7 +2733,7 @@
           <xdr:cNvPr id="12" name="Shape 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000C000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2844,7 +2836,7 @@
           <xdr:cNvPr id="13" name="Shape 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2866,7 +2858,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2945,7 +2937,7 @@
         <xdr:cNvPr id="17" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2964,7 +2956,7 @@
           <xdr:cNvPr id="15" name="Shape 15">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000F000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3067,7 +3059,7 @@
           <xdr:cNvPr id="16" name="Shape 16">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000010000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3089,7 +3081,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3173,7 +3165,7 @@
         <xdr:cNvPr id="19" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4303,16 +4295,16 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="20.375" style="1" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>193</v>
       </c>
@@ -4329,14 +4321,14 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>198</v>
       </c>
@@ -4353,7 +4345,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>203</v>
       </c>
@@ -4370,7 +4362,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>208</v>
       </c>
@@ -4387,28 +4379,28 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4419,7 +4411,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4445,16 +4437,16 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="44" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" style="44" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" style="44" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="44" customWidth="1"/>
+    <col min="3" max="3" width="49.375" style="44" customWidth="1"/>
     <col min="4" max="5" width="11" style="44" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>216</v>
       </c>
@@ -4467,7 +4459,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>155</v>
       </c>
@@ -4480,7 +4472,7 @@
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
         <v>220</v>
       </c>
@@ -4493,7 +4485,7 @@
       <c r="D3" s="50"/>
       <c r="E3" s="51"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="47" t="s">
         <v>223</v>
       </c>
@@ -4506,7 +4498,7 @@
       <c r="D4" s="50"/>
       <c r="E4" s="51"/>
     </row>
-    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="47" t="s">
         <v>238</v>
       </c>
@@ -4519,7 +4511,7 @@
       <c r="D5" s="50"/>
       <c r="E5" s="51"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="47" t="s">
         <v>240</v>
       </c>
@@ -4532,7 +4524,7 @@
       <c r="D6" s="50"/>
       <c r="E6" s="51"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
         <v>242</v>
       </c>
@@ -4545,7 +4537,7 @@
       <c r="D7" s="50"/>
       <c r="E7" s="51"/>
     </row>
-    <row r="8" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52" t="s">
         <v>185</v>
       </c>
@@ -4558,7 +4550,7 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
@@ -4571,7 +4563,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>163</v>
       </c>
@@ -4584,7 +4576,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>166</v>
       </c>
@@ -4597,7 +4589,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>169</v>
       </c>
@@ -4610,7 +4602,7 @@
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
     </row>
-    <row r="13" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="47" t="s">
         <v>245</v>
       </c>
@@ -4623,7 +4615,7 @@
       <c r="D13" s="50"/>
       <c r="E13" s="51"/>
     </row>
-    <row r="14" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="55" t="s">
         <v>64</v>
       </c>
@@ -4636,7 +4628,7 @@
       <c r="D14" s="57"/>
       <c r="E14" s="57"/>
     </row>
-    <row r="15" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="47" t="s">
         <v>247</v>
       </c>
@@ -4649,7 +4641,7 @@
       <c r="D15" s="50"/>
       <c r="E15" s="51"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="55" t="s">
         <v>68</v>
       </c>
@@ -4662,7 +4654,7 @@
       <c r="D16" s="57"/>
       <c r="E16" s="57"/>
     </row>
-    <row r="17" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="47" t="s">
         <v>250</v>
       </c>
@@ -4675,7 +4667,7 @@
       <c r="D17" s="50"/>
       <c r="E17" s="51"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="52" t="s">
         <v>72</v>
       </c>
@@ -4688,7 +4680,7 @@
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -4701,7 +4693,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>78</v>
       </c>
@@ -4714,7 +4706,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>81</v>
       </c>
@@ -4727,7 +4719,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
@@ -4740,7 +4732,7 @@
       <c r="D22" s="46"/>
       <c r="E22" s="46"/>
     </row>
-    <row r="23" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="47" t="s">
         <v>252</v>
       </c>
@@ -4753,7 +4745,7 @@
       <c r="D23" s="50"/>
       <c r="E23" s="51"/>
     </row>
-    <row r="24" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="55" t="s">
         <v>25</v>
       </c>
@@ -4766,7 +4758,7 @@
       <c r="D24" s="57"/>
       <c r="E24" s="57"/>
     </row>
-    <row r="25" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="47" t="s">
         <v>254</v>
       </c>
@@ -4779,7 +4771,7 @@
       <c r="D25" s="50"/>
       <c r="E25" s="51"/>
     </row>
-    <row r="26" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="47" t="s">
         <v>256</v>
       </c>
@@ -4792,7 +4784,7 @@
       <c r="D26" s="50"/>
       <c r="E26" s="51"/>
     </row>
-    <row r="27" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="47" t="s">
         <v>258</v>
       </c>
@@ -4805,7 +4797,7 @@
       <c r="D27" s="50"/>
       <c r="E27" s="51"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="55" t="s">
         <v>108</v>
       </c>
@@ -4818,7 +4810,7 @@
       <c r="D28" s="57"/>
       <c r="E28" s="57"/>
     </row>
-    <row r="29" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="47" t="s">
         <v>260</v>
       </c>
@@ -4831,7 +4823,7 @@
       <c r="D29" s="50"/>
       <c r="E29" s="51"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="55" t="s">
         <v>33</v>
       </c>
@@ -4844,7 +4836,7 @@
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="47" t="s">
         <v>262</v>
       </c>
@@ -4857,7 +4849,7 @@
       <c r="D31" s="50"/>
       <c r="E31" s="51"/>
     </row>
-    <row r="32" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="55" t="s">
         <v>37</v>
       </c>
@@ -4870,7 +4862,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="47" t="s">
         <v>264</v>
       </c>
@@ -4883,7 +4875,7 @@
       <c r="D33" s="50"/>
       <c r="E33" s="51"/>
     </row>
-    <row r="34" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="47" t="s">
         <v>266</v>
       </c>
@@ -4896,7 +4888,7 @@
       <c r="D34" s="50"/>
       <c r="E34" s="51"/>
     </row>
-    <row r="35" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="47" t="s">
         <v>268</v>
       </c>
@@ -4909,7 +4901,7 @@
       <c r="D35" s="50"/>
       <c r="E35" s="51"/>
     </row>
-    <row r="36" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="47" t="s">
         <v>270</v>
       </c>
@@ -4922,7 +4914,7 @@
       <c r="D36" s="50"/>
       <c r="E36" s="51"/>
     </row>
-    <row r="37" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="47" t="s">
         <v>272</v>
       </c>
@@ -4935,7 +4927,7 @@
       <c r="D37" s="50"/>
       <c r="E37" s="51"/>
     </row>
-    <row r="38" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="47" t="s">
         <v>274</v>
       </c>
@@ -4948,7 +4940,7 @@
       <c r="D38" s="50"/>
       <c r="E38" s="51"/>
     </row>
-    <row r="39" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="47" t="s">
         <v>276</v>
       </c>
@@ -4961,7 +4953,7 @@
       <c r="D39" s="50"/>
       <c r="E39" s="51"/>
     </row>
-    <row r="40" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="47" t="s">
         <v>278</v>
       </c>
@@ -4974,7 +4966,7 @@
       <c r="D40" s="50"/>
       <c r="E40" s="51"/>
     </row>
-    <row r="41" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="47" t="s">
         <v>280</v>
       </c>
@@ -4987,7 +4979,7 @@
       <c r="D41" s="50"/>
       <c r="E41" s="51"/>
     </row>
-    <row r="42" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="55" t="s">
         <v>57</v>
       </c>
@@ -5000,7 +4992,7 @@
       <c r="D42" s="57"/>
       <c r="E42" s="57"/>
     </row>
-    <row r="43" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="58" t="s">
         <v>282</v>
       </c>
@@ -5026,21 +5018,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="7.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="7.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.375" style="5" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>215</v>
       </c>
@@ -5057,14 +5049,14 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -5083,7 +5075,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -5100,7 +5092,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -5119,7 +5111,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -5136,7 +5128,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -5155,7 +5147,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -5174,14 +5166,14 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>2</v>
       </c>
@@ -5200,7 +5192,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>2</v>
       </c>
@@ -5219,7 +5211,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>2</v>
       </c>
@@ -5238,7 +5230,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>2</v>
       </c>
@@ -5257,7 +5249,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>2</v>
       </c>
@@ -5273,10 +5265,10 @@
         <v>244</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>2</v>
       </c>
@@ -5292,17 +5284,17 @@
         <v>244</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>3</v>
       </c>
@@ -5321,7 +5313,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>3</v>
       </c>
@@ -5340,7 +5332,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>3</v>
       </c>
@@ -5352,10 +5344,14 @@
         <f>Stories!B33</f>
         <v>List multiple births</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D19" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>3</v>
       </c>
@@ -5367,10 +5363,14 @@
         <f>Stories!B34</f>
         <v>List orphans</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D20" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>3</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>3</v>
       </c>
@@ -5408,14 +5408,14 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>4</v>
       </c>
@@ -5430,7 +5430,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>4</v>
       </c>
@@ -5445,7 +5445,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>4</v>
       </c>
@@ -5460,7 +5460,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>4</v>
       </c>
@@ -5475,7 +5475,7 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>4</v>
       </c>
@@ -5490,7 +5490,7 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>4</v>
       </c>
@@ -5520,19 +5520,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="8" customWidth="1"/>
     <col min="7" max="8" width="11" style="8" customWidth="1"/>
     <col min="9" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>284</v>
       </c>
@@ -5544,7 +5544,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>285</v>
       </c>
@@ -5556,7 +5556,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>286</v>
       </c>
@@ -5568,7 +5568,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -5578,7 +5578,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>287</v>
       </c>
@@ -5590,7 +5590,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>288</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -5612,7 +5612,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>137</v>
       </c>
@@ -5624,7 +5624,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -5634,7 +5634,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5644,7 +5644,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -5654,7 +5654,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5664,7 +5664,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -5674,7 +5674,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>215</v>
       </c>
@@ -5698,7 +5698,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>144</v>
       </c>
@@ -5716,7 +5716,7 @@
       <c r="G15" s="17"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>145</v>
       </c>
@@ -5742,7 +5742,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>146</v>
       </c>
@@ -5768,7 +5768,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>147</v>
       </c>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>148</v>
       </c>
@@ -5820,7 +5820,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="3"/>
       <c r="C20" s="20"/>
@@ -5830,7 +5830,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -5840,7 +5840,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5850,7 +5850,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5860,7 +5860,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5870,7 +5870,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5880,7 +5880,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5890,7 +5890,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5900,7 +5900,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5910,7 +5910,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5920,7 +5920,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5930,7 +5930,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5940,7 +5940,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5950,7 +5950,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5960,7 +5960,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5970,7 +5970,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5980,7 +5980,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5990,7 +5990,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6000,7 +6000,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6010,7 +6010,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -6038,19 +6038,19 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="22" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="12.375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="7.125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="22" customWidth="1"/>
     <col min="7" max="7" width="11" style="22" customWidth="1"/>
     <col min="8" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>138</v>
       </c>
@@ -6071,7 +6071,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23">
         <v>41431</v>
       </c>
@@ -6086,7 +6086,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>41446</v>
       </c>
@@ -6111,7 +6111,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>41459</v>
       </c>
@@ -6122,7 +6122,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6131,7 +6131,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6140,7 +6140,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6149,7 +6149,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>149</v>
       </c>
@@ -6160,7 +6160,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -6169,7 +6169,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -6178,7 +6178,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -6187,7 +6187,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6196,7 +6196,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6205,7 +6205,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -6214,7 +6214,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -6223,7 +6223,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6232,7 +6232,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -6241,7 +6241,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6250,7 +6250,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6259,7 +6259,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6268,7 +6268,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6277,7 +6277,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6286,7 +6286,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6295,7 +6295,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6304,7 +6304,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6313,7 +6313,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6338,21 +6338,21 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="11.625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="23.875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="12.875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="28" customWidth="1"/>
     <col min="5" max="5" width="12" style="28" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="28" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="11.375" style="28" customWidth="1"/>
+    <col min="7" max="7" width="8.375" style="28" customWidth="1"/>
+    <col min="8" max="8" width="9.375" style="28" customWidth="1"/>
     <col min="9" max="9" width="11" style="28" customWidth="1"/>
     <col min="10" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>155</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>159</v>
       </c>
@@ -6427,7 +6427,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="33"/>
       <c r="C4" s="3"/>
@@ -6438,7 +6438,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>220</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>290</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="33"/>
       <c r="C7" s="3"/>
@@ -6489,7 +6489,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>223</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>294</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>296</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="33"/>
       <c r="C11" s="3"/>
@@ -6561,7 +6561,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>238</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>300</v>
       </c>
@@ -6603,7 +6603,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>302</v>
       </c>
@@ -6624,7 +6624,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="33"/>
       <c r="C15" s="3"/>
@@ -6635,7 +6635,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>174</v>
       </c>
@@ -6677,7 +6677,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>176</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>178</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>180</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="33"/>
       <c r="C21" s="3"/>
@@ -6751,7 +6751,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>242</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>41431</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>183</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>41431</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="33"/>
       <c r="C24" s="3"/>
@@ -6804,7 +6804,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>185</v>
       </c>
@@ -6825,7 +6825,7 @@
         <v>41428</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>187</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>41428</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="33"/>
       <c r="C27" s="3"/>
@@ -6857,7 +6857,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="33"/>
       <c r="C28" s="3"/>
@@ -6868,7 +6868,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="33"/>
       <c r="C29" s="3"/>
@@ -6879,7 +6879,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="33"/>
       <c r="C30" s="3"/>
@@ -6890,7 +6890,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="33"/>
       <c r="C31" s="3"/>
@@ -6901,7 +6901,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="33"/>
       <c r="C32" s="3"/>
@@ -6912,7 +6912,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="29" t="s">
         <v>189</v>
@@ -6925,7 +6925,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="29"/>
       <c r="C34" s="3"/>
@@ -6936,7 +6936,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="29" t="s">
         <v>190</v>
@@ -6949,7 +6949,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="7" t="s">
         <v>191</v>
@@ -6962,7 +6962,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="7" t="s">
         <v>192</v>
@@ -6975,7 +6975,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="7" t="s">
         <v>86</v>
@@ -6988,7 +6988,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="7" t="s">
         <v>87</v>
@@ -7001,7 +7001,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="33"/>
       <c r="C40" s="3"/>
@@ -7012,7 +7012,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="29" t="s">
         <v>88</v>
@@ -7042,20 +7042,20 @@
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="34" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="34" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="34" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="34" customWidth="1"/>
+    <col min="2" max="2" width="24.375" style="34" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="34" customWidth="1"/>
     <col min="4" max="4" width="11" style="34" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="8.375" style="34" customWidth="1"/>
     <col min="6" max="6" width="9" style="34" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="34" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="8.375" style="34" customWidth="1"/>
+    <col min="8" max="8" width="9.375" style="34" customWidth="1"/>
     <col min="9" max="256" width="11" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="35"/>
       <c r="B2" s="29"/>
       <c r="C2" s="35"/>
@@ -7095,7 +7095,7 @@
       <c r="H2" s="36"/>
       <c r="I2" s="37"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="str">
         <f>Backlog!B3</f>
         <v>US02</v>
@@ -7126,7 +7126,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>290</v>
       </c>
@@ -7141,7 +7141,7 @@
       <c r="H4" s="36"/>
       <c r="I4" s="37"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>91</v>
       </c>
@@ -7156,7 +7156,7 @@
       <c r="H5" s="36"/>
       <c r="I5" s="37"/>
     </row>
-    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>93</v>
       </c>
@@ -7171,7 +7171,7 @@
       <c r="H6" s="36"/>
       <c r="I6" s="37"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="3"/>
@@ -7182,7 +7182,7 @@
       <c r="H7" s="36"/>
       <c r="I7" s="37"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>223</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>294</v>
       </c>
@@ -7226,7 +7226,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="40"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>296</v>
       </c>
@@ -7241,7 +7241,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="40"/>
     </row>
-    <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>96</v>
       </c>
@@ -7256,7 +7256,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="40"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="33"/>
       <c r="C12" s="3"/>
@@ -7267,7 +7267,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="40"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="str">
         <f>Backlog!B5</f>
         <v>US04</v>
@@ -7298,7 +7298,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>300</v>
       </c>
@@ -7313,7 +7313,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="40"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>302</v>
       </c>
@@ -7328,7 +7328,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="40"/>
     </row>
-    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
@@ -7343,7 +7343,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="40"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="33"/>
       <c r="C17" s="3"/>
@@ -7354,7 +7354,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="40"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>240</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>174</v>
       </c>
@@ -7398,7 +7398,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="40"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>176</v>
       </c>
@@ -7413,7 +7413,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="40"/>
     </row>
-    <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>178</v>
       </c>
@@ -7428,7 +7428,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="40"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="33"/>
       <c r="C22" s="3"/>
@@ -7439,7 +7439,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="40"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="str">
         <f>Backlog!B7</f>
         <v>US06</v>
@@ -7470,7 +7470,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>183</v>
       </c>
@@ -7485,7 +7485,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="40"/>
     </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>104</v>
       </c>
@@ -7500,7 +7500,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="40"/>
     </row>
-    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>106</v>
       </c>
@@ -7515,7 +7515,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="40"/>
     </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="3"/>
@@ -7526,7 +7526,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="40"/>
     </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="str">
         <f>Backlog!B8</f>
         <v>US12</v>
@@ -7557,7 +7557,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>225</v>
       </c>
@@ -7572,7 +7572,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="40"/>
     </row>
-    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>227</v>
       </c>
@@ -7587,7 +7587,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="40"/>
     </row>
-    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>229</v>
       </c>
@@ -7602,7 +7602,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="40"/>
     </row>
-    <row r="32" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>231</v>
       </c>
@@ -7617,7 +7617,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>233</v>
       </c>
@@ -7632,7 +7632,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="7"/>
       <c r="C34" s="3"/>
@@ -7643,7 +7643,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="29" t="s">
         <v>189</v>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="29"/>
       <c r="C36" s="3"/>
@@ -7673,7 +7673,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="29" t="s">
         <v>190</v>
@@ -7686,7 +7686,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="7" t="s">
         <v>235</v>
@@ -7699,7 +7699,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="7" t="s">
         <v>236</v>
@@ -7712,7 +7712,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="66" t="s">
         <v>17</v>
@@ -7972,7 +7972,7 @@
       <c r="IU40" s="44"/>
       <c r="IV40" s="44"/>
     </row>
-    <row r="41" spans="1:256" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:256" ht="59.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="33" t="s">
         <v>62</v>
@@ -7985,7 +7985,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="29" t="s">
         <v>88</v>
@@ -7998,7 +7998,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="1:256" ht="89.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:256" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="33" t="s">
         <v>111</v>
@@ -8011,7 +8011,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="1:256" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:256" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="33" t="s">
         <v>112</v>
@@ -8024,7 +8024,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="33" t="s">
         <v>113</v>
@@ -8037,7 +8037,7 @@
       <c r="H45" s="3"/>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="33" t="s">
         <v>61</v>
@@ -8297,7 +8297,7 @@
       <c r="IU46" s="44"/>
       <c r="IV46" s="44"/>
     </row>
-    <row r="47" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="33" t="s">
         <v>18</v>
@@ -8570,18 +8570,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV33"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="41" customWidth="1"/>
     <col min="2" max="2" width="18" style="41" customWidth="1"/>
     <col min="3" max="256" width="11" style="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -8610,7 +8610,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>247</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>115</v>
       </c>
@@ -8657,7 +8657,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>117</v>
       </c>
@@ -8674,7 +8674,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>119</v>
       </c>
@@ -8691,7 +8691,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="33"/>
       <c r="C6" s="3"/>
@@ -8702,7 +8702,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>250</v>
       </c>
@@ -8732,7 +8732,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>121</v>
       </c>
@@ -8747,7 +8747,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>123</v>
       </c>
@@ -8762,7 +8762,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
@@ -8777,7 +8777,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="33"/>
       <c r="C11" s="3"/>
@@ -8788,7 +8788,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>252</v>
       </c>
@@ -8817,7 +8817,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>127</v>
       </c>
@@ -8832,7 +8832,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>129</v>
       </c>
@@ -8847,7 +8847,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="67" t="s">
         <v>19</v>
       </c>
@@ -9109,7 +9109,7 @@
       <c r="IU15" s="44"/>
       <c r="IV15" s="44"/>
     </row>
-    <row r="16" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="33"/>
       <c r="C16" s="3"/>
@@ -9120,7 +9120,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>254</v>
       </c>
@@ -9149,7 +9149,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="18" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>131</v>
       </c>
@@ -9164,7 +9164,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>132</v>
       </c>
@@ -9179,7 +9179,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="67" t="s">
         <v>20</v>
       </c>
@@ -9441,7 +9441,7 @@
       <c r="IU20" s="44"/>
       <c r="IV20" s="44"/>
     </row>
-    <row r="21" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="35"/>
       <c r="B21" s="33"/>
       <c r="C21" s="3"/>
@@ -9452,7 +9452,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>256</v>
       </c>
@@ -9471,9 +9471,15 @@
       <c r="F22" s="6">
         <v>30</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="G22" s="3">
+        <v>25</v>
+      </c>
+      <c r="H22" s="3">
+        <v>30</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>303</v>
+      </c>
       <c r="J22" s="44"/>
       <c r="K22" s="44"/>
       <c r="L22" s="44"/>
@@ -9722,7 +9728,7 @@
       <c r="IU22" s="44"/>
       <c r="IV22" s="44"/>
     </row>
-    <row r="23" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -9984,7 +9990,7 @@
       <c r="IU23" s="44"/>
       <c r="IV23" s="44"/>
     </row>
-    <row r="24" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -10246,7 +10252,7 @@
       <c r="IU24" s="44"/>
       <c r="IV24" s="44"/>
     </row>
-    <row r="25" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="67" t="s">
         <v>21</v>
       </c>
@@ -10508,7 +10514,7 @@
       <c r="IU25" s="44"/>
       <c r="IV25" s="44"/>
     </row>
-    <row r="26" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="64"/>
       <c r="C26" s="3"/>
@@ -10766,7 +10772,7 @@
       <c r="IU26" s="44"/>
       <c r="IV26" s="44"/>
     </row>
-    <row r="27" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>258</v>
       </c>
@@ -10785,9 +10791,15 @@
       <c r="F27" s="6">
         <v>30</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="G27" s="3">
+        <v>25</v>
+      </c>
+      <c r="H27" s="3">
+        <v>35</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>303</v>
+      </c>
       <c r="J27" s="44"/>
       <c r="K27" s="44"/>
       <c r="L27" s="44"/>
@@ -11036,7 +11048,7 @@
       <c r="IU27" s="44"/>
       <c r="IV27" s="44"/>
     </row>
-    <row r="28" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
@@ -11298,7 +11310,7 @@
       <c r="IU28" s="44"/>
       <c r="IV28" s="44"/>
     </row>
-    <row r="29" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -11560,7 +11572,7 @@
       <c r="IU29" s="44"/>
       <c r="IV29" s="44"/>
     </row>
-    <row r="30" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -11822,7 +11834,7 @@
       <c r="IU30" s="44"/>
       <c r="IV30" s="44"/>
     </row>
-    <row r="31" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -12084,7 +12096,7 @@
       <c r="IU31" s="44"/>
       <c r="IV31" s="44"/>
     </row>
-    <row r="32" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="67" t="s">
         <v>22</v>
       </c>
@@ -12346,7 +12358,7 @@
       <c r="IU32" s="44"/>
       <c r="IV32" s="44"/>
     </row>
-    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="64"/>
       <c r="C33" s="3"/>
@@ -12621,14 +12633,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="42" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="42" customWidth="1"/>
+    <col min="2" max="2" width="21.125" style="42" customWidth="1"/>
     <col min="3" max="256" width="11" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -12657,7 +12669,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="68" t="str">
         <f>Backlog!$B$17</f>
         <v>US28</v>
@@ -12682,7 +12694,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
         <v>305</v>
       </c>
@@ -12944,7 +12956,7 @@
       <c r="IU3" s="44"/>
       <c r="IV3" s="44"/>
     </row>
-    <row r="4" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="70" t="s">
         <v>306</v>
       </c>
@@ -13206,7 +13218,7 @@
       <c r="IU4" s="44"/>
       <c r="IV4" s="44"/>
     </row>
-    <row r="5" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="70" t="s">
         <v>310</v>
       </c>
@@ -13468,7 +13480,7 @@
       <c r="IU5" s="44"/>
       <c r="IV5" s="44"/>
     </row>
-    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="70"/>
       <c r="B6" s="70"/>
       <c r="C6" s="69"/>
@@ -13726,7 +13738,7 @@
       <c r="IU6" s="44"/>
       <c r="IV6" s="44"/>
     </row>
-    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="str">
         <f>Backlog!$B$18</f>
         <v>US30</v>
@@ -13751,7 +13763,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="69" t="s">
         <v>309</v>
       </c>
@@ -13766,7 +13778,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="69" t="s">
         <v>314</v>
       </c>
@@ -13781,7 +13793,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="69" t="s">
         <v>315</v>
       </c>
@@ -13796,7 +13808,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -13807,7 +13819,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -13818,7 +13830,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -13829,7 +13841,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -13856,13 +13868,13 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="9" width="11" style="43" customWidth="1"/>
     <col min="10" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>216</v>
       </c>
@@ -13891,7 +13903,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -13902,7 +13914,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -13913,7 +13925,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -13924,7 +13936,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -13935,7 +13947,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -13946,7 +13958,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -13957,7 +13969,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -13968,7 +13980,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -13979,7 +13991,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>

</xml_diff>

<commit_message>
Sprint3- US34 and US35
US34 and US35 complete.  Team Report updated.  Gedcom file altered to demonstrate US34 and US35 output.  Added unit tests but cannot get TestFile.py to run.
</commit_message>
<xml_diff>
--- a/TeamNick_Jeremy_AmieReport.xlsx
+++ b/TeamNick_Jeremy_AmieReport.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickcohron/Stevens/Agile Methods/Project/AgileMethods/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14640" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21600" windowHeight="14640" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -18,9 +23,12 @@
     <sheet name="Sprint4" sheetId="9" r:id="rId9"/>
     <sheet name="Stories" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -28,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="352">
   <si>
     <t>All individual IDs should be unique and all family IDs should be unique</t>
   </si>
@@ -1133,17 +1141,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="m/d"/>
-    <numFmt numFmtId="170" formatCode="@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1194,6 +1197,12 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -1392,8 +1401,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1415,16 +1425,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1436,7 +1446,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1445,7 +1455,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1454,7 +1464,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1504,13 +1514,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1594,7 +1605,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1611,6 +1630,7 @@
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1692,23 +1712,36 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F845-4DB0-BF4B-61C3F2B72AD9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="510881320"/>
-        <c:axId val="510793576"/>
+        <c:smooth val="0"/>
+        <c:axId val="-925857664"/>
+        <c:axId val="-1005852464"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="510881320"/>
+        <c:axId val="-925857664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
         <c:spPr>
           <a:ln w="12700" cap="flat">
@@ -1734,17 +1767,18 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="510793576"/>
+        <c:crossAx val="-1005852464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="510793576"/>
+        <c:axId val="-1005852464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1758,6 +1792,8 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="12700" cap="flat">
@@ -1783,7 +1819,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="510881320"/>
+        <c:crossAx val="-925857664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7.5"/>
@@ -1829,7 +1865,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1846,6 +1890,7 @@
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1915,23 +1960,36 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-60FF-4851-ABD9-FA91BB13A616}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="283067848"/>
-        <c:axId val="282651544"/>
+        <c:smooth val="0"/>
+        <c:axId val="-925135392"/>
+        <c:axId val="-925132912"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="283067848"/>
+        <c:axId val="-925135392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
         <c:spPr>
           <a:ln w="12700" cap="flat">
@@ -1957,17 +2015,18 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="282651544"/>
+        <c:crossAx val="-925132912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="282651544"/>
+        <c:axId val="-925132912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1981,6 +2040,8 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="12700" cap="flat">
@@ -2006,7 +2067,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="283067848"/>
+        <c:crossAx val="-925135392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="6.0"/>
@@ -2068,7 +2129,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2104,7 +2165,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2123,7 +2184,7 @@
           <xdr:cNvPr id="3" name="Shape 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2226,7 +2287,7 @@
           <xdr:cNvPr id="4" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2248,7 +2309,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2327,7 +2388,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2346,7 +2407,7 @@
           <xdr:cNvPr id="6" name="Shape 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2449,7 +2510,7 @@
           <xdr:cNvPr id="7" name="Shape 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2471,7 +2532,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2550,7 +2611,7 @@
         <xdr:cNvPr id="11" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2569,7 +2630,7 @@
           <xdr:cNvPr id="9" name="Shape 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2672,7 +2733,7 @@
           <xdr:cNvPr id="10" name="Shape 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2694,7 +2755,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2820,7 +2881,7 @@
         <xdr:cNvPr id="14" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2839,7 +2900,7 @@
           <xdr:cNvPr id="12" name="Shape 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000C000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2942,7 +3003,7 @@
           <xdr:cNvPr id="13" name="Shape 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2964,7 +3025,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3043,7 +3104,7 @@
         <xdr:cNvPr id="17" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3062,7 +3123,7 @@
           <xdr:cNvPr id="15" name="Shape 15">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000F000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3165,7 +3226,7 @@
           <xdr:cNvPr id="16" name="Shape 16">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000010000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3187,7 +3248,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3271,7 +3332,7 @@
         <xdr:cNvPr id="19" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4396,21 +4457,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="20.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
+    <col min="4" max="5" width="20.5" style="1" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>269</v>
       </c>
@@ -4427,14 +4488,14 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>274</v>
       </c>
@@ -4451,7 +4512,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>279</v>
       </c>
@@ -4468,7 +4529,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>284</v>
       </c>
@@ -4485,28 +4546,28 @@
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4517,7 +4578,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4532,32 +4593,27 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView showGridLines="0" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="44" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="44" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="44" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" style="44" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="44" customWidth="1"/>
     <col min="4" max="5" width="11" style="44" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>292</v>
       </c>
@@ -4570,7 +4626,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="31.5" customHeight="1">
+    <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>211</v>
       </c>
@@ -4583,7 +4639,7 @@
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="47" t="s">
         <v>296</v>
       </c>
@@ -4596,7 +4652,7 @@
       <c r="D3" s="50"/>
       <c r="E3" s="51"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="47" t="s">
         <v>299</v>
       </c>
@@ -4609,7 +4665,7 @@
       <c r="D4" s="50"/>
       <c r="E4" s="51"/>
     </row>
-    <row r="5" spans="1:5" ht="31.5" customHeight="1">
+    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="47" t="s">
         <v>146</v>
       </c>
@@ -4622,7 +4678,7 @@
       <c r="D5" s="50"/>
       <c r="E5" s="51"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="47" t="s">
         <v>148</v>
       </c>
@@ -4635,7 +4691,7 @@
       <c r="D6" s="50"/>
       <c r="E6" s="51"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="47" t="s">
         <v>150</v>
       </c>
@@ -4648,7 +4704,7 @@
       <c r="D7" s="50"/>
       <c r="E7" s="51"/>
     </row>
-    <row r="8" spans="1:5" ht="47.25" customHeight="1">
+    <row r="8" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="52" t="s">
         <v>261</v>
       </c>
@@ -4661,7 +4717,7 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="1:5" ht="31.5" customHeight="1">
+    <row r="9" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
@@ -4674,7 +4730,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="31.5" customHeight="1">
+    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>219</v>
       </c>
@@ -4687,7 +4743,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="31.5" customHeight="1">
+    <row r="11" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>88</v>
       </c>
@@ -4700,7 +4756,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="31.5" customHeight="1">
+    <row r="12" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
         <v>91</v>
       </c>
@@ -4713,7 +4769,7 @@
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
     </row>
-    <row r="13" spans="1:5" ht="47.25" customHeight="1">
+    <row r="13" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="47" t="s">
         <v>153</v>
       </c>
@@ -4726,7 +4782,7 @@
       <c r="D13" s="50"/>
       <c r="E13" s="51"/>
     </row>
-    <row r="14" spans="1:5" ht="63" customHeight="1">
+    <row r="14" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="55" t="s">
         <v>26</v>
       </c>
@@ -4739,7 +4795,7 @@
       <c r="D14" s="57"/>
       <c r="E14" s="57"/>
     </row>
-    <row r="15" spans="1:5" ht="31.5" customHeight="1">
+    <row r="15" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="47" t="s">
         <v>155</v>
       </c>
@@ -4752,7 +4808,7 @@
       <c r="D15" s="50"/>
       <c r="E15" s="51"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="55" t="s">
         <v>30</v>
       </c>
@@ -4765,7 +4821,7 @@
       <c r="D16" s="57"/>
       <c r="E16" s="57"/>
     </row>
-    <row r="17" spans="1:5" ht="31.5" customHeight="1">
+    <row r="17" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="47" t="s">
         <v>158</v>
       </c>
@@ -4778,7 +4834,7 @@
       <c r="D17" s="50"/>
       <c r="E17" s="51"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="52" t="s">
         <v>34</v>
       </c>
@@ -4791,7 +4847,7 @@
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>106</v>
       </c>
@@ -4804,7 +4860,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>109</v>
       </c>
@@ -4817,7 +4873,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="31.5" customHeight="1">
+    <row r="21" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>112</v>
       </c>
@@ -4830,7 +4886,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="31.5" customHeight="1">
+    <row r="22" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
         <v>115</v>
       </c>
@@ -4843,7 +4899,7 @@
       <c r="D22" s="46"/>
       <c r="E22" s="46"/>
     </row>
-    <row r="23" spans="1:5" ht="31.5" customHeight="1">
+    <row r="23" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="47" t="s">
         <v>160</v>
       </c>
@@ -4856,7 +4912,7 @@
       <c r="D23" s="50"/>
       <c r="E23" s="51"/>
     </row>
-    <row r="24" spans="1:5" ht="31.5" customHeight="1">
+    <row r="24" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="55" t="s">
         <v>1</v>
       </c>
@@ -4869,7 +4925,7 @@
       <c r="D24" s="57"/>
       <c r="E24" s="57"/>
     </row>
-    <row r="25" spans="1:5" ht="47.25" customHeight="1">
+    <row r="25" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="47" t="s">
         <v>162</v>
       </c>
@@ -4882,7 +4938,7 @@
       <c r="D25" s="50"/>
       <c r="E25" s="51"/>
     </row>
-    <row r="26" spans="1:5" ht="31.5" customHeight="1">
+    <row r="26" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="47" t="s">
         <v>164</v>
       </c>
@@ -4895,7 +4951,7 @@
       <c r="D26" s="50"/>
       <c r="E26" s="51"/>
     </row>
-    <row r="27" spans="1:5" ht="126" customHeight="1">
+    <row r="27" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="47" t="s">
         <v>166</v>
       </c>
@@ -4908,7 +4964,7 @@
       <c r="D27" s="50"/>
       <c r="E27" s="51"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="55" t="s">
         <v>60</v>
       </c>
@@ -4921,7 +4977,7 @@
       <c r="D28" s="57"/>
       <c r="E28" s="57"/>
     </row>
-    <row r="29" spans="1:5" ht="31.5" customHeight="1">
+    <row r="29" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="47" t="s">
         <v>168</v>
       </c>
@@ -4934,7 +4990,7 @@
       <c r="D29" s="50"/>
       <c r="E29" s="51"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="55" t="s">
         <v>8</v>
       </c>
@@ -4947,7 +5003,7 @@
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="47" t="s">
         <v>170</v>
       </c>
@@ -4960,7 +5016,7 @@
       <c r="D31" s="50"/>
       <c r="E31" s="51"/>
     </row>
-    <row r="32" spans="1:5" ht="31.5" customHeight="1">
+    <row r="32" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="55" t="s">
         <v>12</v>
       </c>
@@ -4973,7 +5029,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="47" t="s">
         <v>172</v>
       </c>
@@ -4986,7 +5042,7 @@
       <c r="D33" s="50"/>
       <c r="E33" s="51"/>
     </row>
-    <row r="34" spans="1:5" ht="31.5" customHeight="1">
+    <row r="34" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="47" t="s">
         <v>174</v>
       </c>
@@ -4999,7 +5055,7 @@
       <c r="D34" s="50"/>
       <c r="E34" s="51"/>
     </row>
-    <row r="35" spans="1:5" ht="47.25" customHeight="1">
+    <row r="35" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="47" t="s">
         <v>176</v>
       </c>
@@ -5012,7 +5068,7 @@
       <c r="D35" s="50"/>
       <c r="E35" s="51"/>
     </row>
-    <row r="36" spans="1:5" ht="31.5" customHeight="1">
+    <row r="36" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="47" t="s">
         <v>178</v>
       </c>
@@ -5025,7 +5081,7 @@
       <c r="D36" s="50"/>
       <c r="E36" s="51"/>
     </row>
-    <row r="37" spans="1:5" ht="31.5" customHeight="1">
+    <row r="37" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="47" t="s">
         <v>333</v>
       </c>
@@ -5038,7 +5094,7 @@
       <c r="D37" s="50"/>
       <c r="E37" s="51"/>
     </row>
-    <row r="38" spans="1:5" ht="31.5" customHeight="1">
+    <row r="38" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="47" t="s">
         <v>335</v>
       </c>
@@ -5051,7 +5107,7 @@
       <c r="D38" s="50"/>
       <c r="E38" s="51"/>
     </row>
-    <row r="39" spans="1:5" ht="31.5" customHeight="1">
+    <row r="39" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="47" t="s">
         <v>337</v>
       </c>
@@ -5064,7 +5120,7 @@
       <c r="D39" s="50"/>
       <c r="E39" s="51"/>
     </row>
-    <row r="40" spans="1:5" ht="31.5" customHeight="1">
+    <row r="40" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="47" t="s">
         <v>339</v>
       </c>
@@ -5077,7 +5133,7 @@
       <c r="D40" s="50"/>
       <c r="E40" s="51"/>
     </row>
-    <row r="41" spans="1:5" ht="31.5" customHeight="1">
+    <row r="41" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="47" t="s">
         <v>341</v>
       </c>
@@ -5090,7 +5146,7 @@
       <c r="D41" s="50"/>
       <c r="E41" s="51"/>
     </row>
-    <row r="42" spans="1:5" ht="31.5" customHeight="1">
+    <row r="42" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="55" t="s">
         <v>19</v>
       </c>
@@ -5103,7 +5159,7 @@
       <c r="D42" s="57"/>
       <c r="E42" s="57"/>
     </row>
-    <row r="43" spans="1:5" ht="31.5" customHeight="1">
+    <row r="43" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="58" t="s">
         <v>343</v>
       </c>
@@ -5115,512 +5171,6 @@
       </c>
       <c r="D43" s="61"/>
       <c r="E43" s="62"/>
-    </row>
-  </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E29"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="5.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="256" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f>Stories!A3</f>
-        <v>US02</v>
-      </c>
-      <c r="C3" s="2" t="str">
-        <f>Stories!B3</f>
-        <v>Birth before marriage</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="6">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f>Stories!A5</f>
-        <v>US04</v>
-      </c>
-      <c r="C5" s="7" t="str">
-        <f>Stories!B5</f>
-        <v>Marriage before divorce</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="6">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="str">
-        <f>Stories!A7</f>
-        <v>US06</v>
-      </c>
-      <c r="C7" s="7" t="str">
-        <f>Stories!B7</f>
-        <v>Divorce before death</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="6">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <f>Stories!A13</f>
-        <v>US12</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f>Stories!B13</f>
-        <v>Parents not too old</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="6">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <f>Stories!A15</f>
-        <v>US14</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f>Stories!B15</f>
-        <v>Multiple births &lt;= 5</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="6">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="str">
-        <f>Stories!A17</f>
-        <v>US16</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <f>Stories!B17</f>
-        <v>Male last names</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="6">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="str">
-        <f>Stories!A23</f>
-        <v>US22</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f>Stories!B23</f>
-        <v>Unique IDs</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="6">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2" t="str">
-        <f>Stories!A25</f>
-        <v>US24</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <f>Stories!B25</f>
-        <v>Unique families by spouses</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="6">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="str">
-        <f>Stories!A26</f>
-        <v>US25</v>
-      </c>
-      <c r="C14" s="2" t="str">
-        <f>Stories!B26</f>
-        <v>Unique first names in families</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
-      <c r="A15" s="6">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2" t="str">
-        <f>Stories!A27</f>
-        <v>US26</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f>Stories!B27</f>
-        <v>Corresponding entries</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1">
-      <c r="A17" s="6">
-        <v>3</v>
-      </c>
-      <c r="B17" s="2" t="str">
-        <f>Stories!A29</f>
-        <v>US28</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f>Stories!B29</f>
-        <v>Order siblings by age</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="6">
-        <v>3</v>
-      </c>
-      <c r="B18" s="2" t="str">
-        <f>Stories!A31</f>
-        <v>US30</v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <f>Stories!B31</f>
-        <v>List living married</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
-      <c r="A19" s="6">
-        <v>3</v>
-      </c>
-      <c r="B19" s="2" t="str">
-        <f>Stories!A33</f>
-        <v>US32</v>
-      </c>
-      <c r="C19" s="2" t="str">
-        <f>Stories!B33</f>
-        <v>List multiple births</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
-      <c r="A20" s="6">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2" t="str">
-        <f>Stories!A34</f>
-        <v>US33</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f>Stories!B34</f>
-        <v>List orphans</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="6">
-        <v>3</v>
-      </c>
-      <c r="B21" s="2" t="str">
-        <f>Stories!A35</f>
-        <v>US34</v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <f>Stories!B35</f>
-        <v>List large age differences</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
-      <c r="A22" s="6">
-        <v>3</v>
-      </c>
-      <c r="B22" s="2" t="str">
-        <f>Stories!A36</f>
-        <v>US35</v>
-      </c>
-      <c r="C22" s="2" t="str">
-        <f>Stories!B36</f>
-        <v>List recent births</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1">
-      <c r="A24" s="6">
-        <v>4</v>
-      </c>
-      <c r="B24" s="2" t="str">
-        <f>Stories!A37</f>
-        <v>US36</v>
-      </c>
-      <c r="C24" s="2" t="str">
-        <f>Stories!B37</f>
-        <v>List recent deaths</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1">
-      <c r="A25" s="6">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2" t="str">
-        <f>Stories!A38</f>
-        <v>US37</v>
-      </c>
-      <c r="C25" s="2" t="str">
-        <f>Stories!B38</f>
-        <v>List recent survivors</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1">
-      <c r="A26" s="6">
-        <v>4</v>
-      </c>
-      <c r="B26" s="2" t="str">
-        <f>Stories!A39</f>
-        <v>US38</v>
-      </c>
-      <c r="C26" s="2" t="str">
-        <f>Stories!B39</f>
-        <v>List upcoming birthdays</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1">
-      <c r="A27" s="6">
-        <v>4</v>
-      </c>
-      <c r="B27" s="2" t="str">
-        <f>Stories!A40</f>
-        <v>US39</v>
-      </c>
-      <c r="C27" s="2" t="str">
-        <f>Stories!B40</f>
-        <v>List upcoming anniversaries</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1">
-      <c r="A28" s="6">
-        <v>4</v>
-      </c>
-      <c r="B28" s="2" t="str">
-        <f>Stories!A41</f>
-        <v>US40</v>
-      </c>
-      <c r="C28" s="2" t="str">
-        <f>Stories!B41</f>
-        <v>Include input line numbers</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1">
-      <c r="A29" s="6">
-        <v>4</v>
-      </c>
-      <c r="B29" s="2" t="str">
-        <f>Stories!A43</f>
-        <v>US42</v>
-      </c>
-      <c r="C29" s="2" t="str">
-        <f>Stories!B43</f>
-        <v>Reject illegitimate dates</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -5628,33 +5178,528 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="5" customWidth="1"/>
+    <col min="6" max="256" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>Stories!A3</f>
+        <v>US02</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>Stories!B3</f>
+        <v>Birth before marriage</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>Stories!A5</f>
+        <v>US04</v>
+      </c>
+      <c r="C5" s="7" t="str">
+        <f>Stories!B5</f>
+        <v>Marriage before divorce</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>Stories!A7</f>
+        <v>US06</v>
+      </c>
+      <c r="C7" s="7" t="str">
+        <f>Stories!B7</f>
+        <v>Divorce before death</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>Stories!A13</f>
+        <v>US12</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>Stories!B13</f>
+        <v>Parents not too old</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="6">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>Stories!A15</f>
+        <v>US14</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f>Stories!B15</f>
+        <v>Multiple births &lt;= 5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>Stories!A17</f>
+        <v>US16</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f>Stories!B17</f>
+        <v>Male last names</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="6">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>Stories!A23</f>
+        <v>US22</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f>Stories!B23</f>
+        <v>Unique IDs</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="6">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>Stories!A25</f>
+        <v>US24</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f>Stories!B25</f>
+        <v>Unique families by spouses</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="6">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>Stories!A26</f>
+        <v>US25</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f>Stories!B26</f>
+        <v>Unique first names in families</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="6">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <f>Stories!A27</f>
+        <v>US26</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f>Stories!B27</f>
+        <v>Corresponding entries</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="6">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>Stories!A29</f>
+        <v>US28</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f>Stories!B29</f>
+        <v>Order siblings by age</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="6">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f>Stories!A31</f>
+        <v>US30</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f>Stories!B31</f>
+        <v>List living married</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="6">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="str">
+        <f>Stories!A33</f>
+        <v>US32</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f>Stories!B33</f>
+        <v>List multiple births</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="6">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f>Stories!A34</f>
+        <v>US33</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f>Stories!B34</f>
+        <v>List orphans</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="6">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f>Stories!A35</f>
+        <v>US34</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f>Stories!B35</f>
+        <v>List large age differences</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f>Stories!A36</f>
+        <v>US35</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f>Stories!B36</f>
+        <v>List recent births</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="6">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f>Stories!A37</f>
+        <v>US36</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f>Stories!B37</f>
+        <v>List recent deaths</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="6">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f>Stories!A38</f>
+        <v>US37</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f>Stories!B38</f>
+        <v>List recent survivors</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="6">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f>Stories!A39</f>
+        <v>US38</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f>Stories!B39</f>
+        <v>List upcoming birthdays</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="6">
+        <v>4</v>
+      </c>
+      <c r="B27" s="2" t="str">
+        <f>Stories!A40</f>
+        <v>US39</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f>Stories!B40</f>
+        <v>List upcoming anniversaries</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="6">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2" t="str">
+        <f>Stories!A41</f>
+        <v>US40</v>
+      </c>
+      <c r="C28" s="2" t="str">
+        <f>Stories!B41</f>
+        <v>Include input line numbers</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f>Stories!A43</f>
+        <v>US42</v>
+      </c>
+      <c r="C29" s="2" t="str">
+        <f>Stories!B43</f>
+        <v>Reject illegitimate dates</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
     <col min="7" max="8" width="11" style="8" customWidth="1"/>
     <col min="9" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>345</v>
       </c>
@@ -5666,7 +5711,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>346</v>
       </c>
@@ -5678,7 +5723,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1">
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>347</v>
       </c>
@@ -5690,7 +5735,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -5700,7 +5745,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1">
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>348</v>
       </c>
@@ -5712,7 +5757,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
         <v>349</v>
       </c>
@@ -5724,7 +5769,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -5734,7 +5779,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>194</v>
       </c>
@@ -5746,7 +5791,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -5756,7 +5801,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5766,7 +5811,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1">
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -5776,7 +5821,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1">
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5786,7 +5831,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1">
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -5796,7 +5841,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1">
+    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>291</v>
       </c>
@@ -5820,7 +5865,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1">
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>201</v>
       </c>
@@ -5838,7 +5883,7 @@
       <c r="G15" s="17"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>202</v>
       </c>
@@ -5864,7 +5909,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1">
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
         <v>203</v>
       </c>
@@ -5890,7 +5935,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1">
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
         <v>204</v>
       </c>
@@ -5916,7 +5961,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1">
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
         <v>205</v>
       </c>
@@ -5942,7 +5987,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1">
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="3"/>
       <c r="C20" s="20"/>
@@ -5952,7 +5997,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -5962,7 +6007,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5972,7 +6017,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1">
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5982,7 +6027,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5992,7 +6037,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1">
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6002,7 +6047,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1">
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6012,7 +6057,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="12.75" customHeight="1">
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6022,7 +6067,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1">
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -6032,7 +6077,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1">
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6042,7 +6087,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1">
+    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6052,7 +6097,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1">
+    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6062,7 +6107,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1">
+    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6072,7 +6117,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1">
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="10"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6082,7 +6127,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1">
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -6092,7 +6137,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1">
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -6102,7 +6147,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1">
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="10"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -6112,7 +6157,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1">
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="10"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6122,7 +6167,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1">
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="10"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6132,7 +6177,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1">
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="10"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -6149,35 +6194,30 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="22" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="22" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="22" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="22" customWidth="1"/>
     <col min="7" max="7" width="11" style="22" customWidth="1"/>
     <col min="8" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75" customHeight="1">
+    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>195</v>
       </c>
@@ -6198,7 +6238,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="12.75" customHeight="1">
+    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="23">
         <v>41431</v>
       </c>
@@ -6213,7 +6253,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="23">
         <v>41446</v>
       </c>
@@ -6238,7 +6278,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>41459</v>
       </c>
@@ -6263,7 +6303,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="12.75" customHeight="1">
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6272,7 +6312,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="12.75" customHeight="1">
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6281,7 +6321,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="12.75" customHeight="1">
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6290,7 +6330,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="12.75" customHeight="1">
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="27" t="s">
         <v>308</v>
       </c>
@@ -6301,7 +6341,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="12.75" customHeight="1">
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -6310,7 +6350,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="12.75" customHeight="1">
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -6319,7 +6359,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="12.75" customHeight="1">
+    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -6328,7 +6368,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="12.75" customHeight="1">
+    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6337,7 +6377,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="12.75" customHeight="1">
+    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6346,7 +6386,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="12.75" customHeight="1">
+    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -6355,7 +6395,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="12.75" customHeight="1">
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -6364,7 +6404,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="12.75" customHeight="1">
+    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6373,7 +6413,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="12.75" customHeight="1">
+    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -6382,7 +6422,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="12.75" customHeight="1">
+    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6391,7 +6431,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="12.75" customHeight="1">
+    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6400,7 +6440,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="12.75" customHeight="1">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6409,7 +6449,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1">
+    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6418,7 +6458,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="12.75" customHeight="1">
+    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6427,7 +6467,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" customHeight="1">
+    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6436,7 +6476,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" customHeight="1">
+    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6445,7 +6485,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="12.75" customHeight="1">
+    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6454,7 +6494,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="12.75" customHeight="1">
+    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6464,42 +6504,36 @@
       <c r="G26" s="3"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="28" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="28" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="28" customWidth="1"/>
     <col min="5" max="5" width="12" style="28" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="28" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="28" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="28" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="28" customWidth="1"/>
     <col min="9" max="9" width="11" style="28" customWidth="1"/>
     <col min="10" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>292</v>
       </c>
@@ -6528,7 +6562,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>211</v>
       </c>
@@ -6555,7 +6589,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25" customHeight="1">
+    <row r="3" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>215</v>
       </c>
@@ -6574,7 +6608,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" s="33"/>
       <c r="C4" s="3"/>
@@ -6585,7 +6619,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5" customHeight="1">
+    <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>296</v>
       </c>
@@ -6604,7 +6638,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" customHeight="1">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>351</v>
       </c>
@@ -6625,7 +6659,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="33"/>
       <c r="C7" s="3"/>
@@ -6636,7 +6670,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="25.5" customHeight="1">
+    <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>299</v>
       </c>
@@ -6655,7 +6689,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="25.5" customHeight="1">
+    <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>224</v>
       </c>
@@ -6676,7 +6710,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="51" customHeight="1">
+    <row r="10" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>226</v>
       </c>
@@ -6697,7 +6731,7 @@
         <v>41426</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="33"/>
       <c r="C11" s="3"/>
@@ -6708,7 +6742,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="25.5" customHeight="1">
+    <row r="12" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>146</v>
       </c>
@@ -6729,7 +6763,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="51" customHeight="1">
+    <row r="13" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>230</v>
       </c>
@@ -6750,7 +6784,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="51" customHeight="1">
+    <row r="14" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>232</v>
       </c>
@@ -6771,7 +6805,7 @@
         <v>41429</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="33"/>
       <c r="C15" s="3"/>
@@ -6782,7 +6816,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="25.5" customHeight="1">
+    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>148</v>
       </c>
@@ -6803,7 +6837,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="38.25" customHeight="1">
+    <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>96</v>
       </c>
@@ -6824,7 +6858,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="38.25" customHeight="1">
+    <row r="18" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>98</v>
       </c>
@@ -6845,7 +6879,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="63.75" customHeight="1">
+    <row r="19" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>100</v>
       </c>
@@ -6866,7 +6900,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="51" customHeight="1">
+    <row r="20" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>102</v>
       </c>
@@ -6887,7 +6921,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1">
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="33"/>
       <c r="C21" s="3"/>
@@ -6898,7 +6932,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="38.25" customHeight="1">
+    <row r="22" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>150</v>
       </c>
@@ -6919,7 +6953,7 @@
         <v>41431</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="38.25" customHeight="1">
+    <row r="23" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>259</v>
       </c>
@@ -6940,7 +6974,7 @@
         <v>41431</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1">
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="33"/>
       <c r="C24" s="3"/>
@@ -6951,7 +6985,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="25.5" customHeight="1">
+    <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>261</v>
       </c>
@@ -6972,7 +7006,7 @@
         <v>41428</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="25.5" customHeight="1">
+    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>263</v>
       </c>
@@ -6993,7 +7027,7 @@
         <v>41428</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1">
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="33"/>
       <c r="C27" s="3"/>
@@ -7004,7 +7038,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1">
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="33"/>
       <c r="C28" s="3"/>
@@ -7015,7 +7049,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" ht="15" customHeight="1">
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="33"/>
       <c r="C29" s="3"/>
@@ -7026,7 +7060,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="15" customHeight="1">
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="33"/>
       <c r="C30" s="3"/>
@@ -7037,7 +7071,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="15" customHeight="1">
+    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="33"/>
       <c r="C31" s="3"/>
@@ -7048,7 +7082,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="1:9" ht="15" customHeight="1">
+    <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="33"/>
       <c r="C32" s="3"/>
@@ -7059,7 +7093,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" ht="15" customHeight="1">
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="29" t="s">
         <v>265</v>
@@ -7072,7 +7106,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="15" customHeight="1">
+    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="29"/>
       <c r="C34" s="3"/>
@@ -7083,7 +7117,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="1:9" ht="15" customHeight="1">
+    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="29" t="s">
         <v>266</v>
@@ -7096,7 +7130,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:9" ht="25.5" customHeight="1">
+    <row r="36" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="7" t="s">
         <v>267</v>
@@ -7109,7 +7143,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="1:9" ht="25.5" customHeight="1">
+    <row r="37" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7" t="s">
         <v>268</v>
@@ -7122,7 +7156,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:9" ht="25.5" customHeight="1">
+    <row r="38" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="7" t="s">
         <v>117</v>
@@ -7135,7 +7169,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:9" ht="25.5" customHeight="1">
+    <row r="39" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7" t="s">
         <v>118</v>
@@ -7148,7 +7182,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" ht="15" customHeight="1">
+    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="33"/>
       <c r="C40" s="3"/>
@@ -7159,7 +7193,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="1:9" ht="15" customHeight="1">
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="29" t="s">
         <v>119</v>
@@ -7173,42 +7207,36 @@
       <c r="I41" s="10"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV47"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="34" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="34" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" style="34" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="34" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="34" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="34" customWidth="1"/>
     <col min="4" max="4" width="11" style="34" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="34" customWidth="1"/>
     <col min="6" max="6" width="9" style="34" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="34" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="34" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="34" customWidth="1"/>
     <col min="9" max="256" width="11" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>292</v>
       </c>
@@ -7237,7 +7265,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="35"/>
       <c r="B2" s="29"/>
       <c r="C2" s="35"/>
@@ -7248,7 +7276,7 @@
       <c r="H2" s="36"/>
       <c r="I2" s="37"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="str">
         <f>Backlog!B3</f>
         <v>US02</v>
@@ -7279,7 +7307,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>351</v>
       </c>
@@ -7294,7 +7322,7 @@
       <c r="H4" s="36"/>
       <c r="I4" s="37"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>122</v>
       </c>
@@ -7309,7 +7337,7 @@
       <c r="H5" s="36"/>
       <c r="I5" s="37"/>
     </row>
-    <row r="6" spans="1:9" ht="25.5" customHeight="1">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>124</v>
       </c>
@@ -7324,7 +7352,7 @@
       <c r="H6" s="36"/>
       <c r="I6" s="37"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="3"/>
@@ -7335,7 +7363,7 @@
       <c r="H7" s="36"/>
       <c r="I7" s="37"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>299</v>
       </c>
@@ -7364,7 +7392,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>224</v>
       </c>
@@ -7379,7 +7407,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="40"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>226</v>
       </c>
@@ -7394,7 +7422,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="40"/>
     </row>
-    <row r="11" spans="1:9" ht="25.5" customHeight="1">
+    <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>127</v>
       </c>
@@ -7409,7 +7437,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="40"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="33"/>
       <c r="C12" s="3"/>
@@ -7420,7 +7448,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="40"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="str">
         <f>Backlog!B5</f>
         <v>US04</v>
@@ -7451,7 +7479,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>230</v>
       </c>
@@ -7466,7 +7494,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="40"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>232</v>
       </c>
@@ -7481,7 +7509,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="40"/>
     </row>
-    <row r="16" spans="1:9" ht="25.5" customHeight="1">
+    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>130</v>
       </c>
@@ -7496,7 +7524,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="40"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1">
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="33"/>
       <c r="C17" s="3"/>
@@ -7507,7 +7535,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="40"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1">
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>148</v>
       </c>
@@ -7536,7 +7564,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="25.5" customHeight="1">
+    <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>96</v>
       </c>
@@ -7551,7 +7579,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="40"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1">
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>98</v>
       </c>
@@ -7566,7 +7594,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="40"/>
     </row>
-    <row r="21" spans="1:9" ht="25.5" customHeight="1">
+    <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -7581,7 +7609,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="40"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1">
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="33"/>
       <c r="C22" s="3"/>
@@ -7592,7 +7620,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="40"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1">
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="str">
         <f>Backlog!B7</f>
         <v>US06</v>
@@ -7623,7 +7651,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1">
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>259</v>
       </c>
@@ -7638,7 +7666,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="40"/>
     </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1">
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>135</v>
       </c>
@@ -7653,7 +7681,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="40"/>
     </row>
-    <row r="26" spans="1:9" ht="25.5" customHeight="1">
+    <row r="26" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>137</v>
       </c>
@@ -7668,7 +7696,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="40"/>
     </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1">
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="3"/>
@@ -7679,7 +7707,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="40"/>
     </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1">
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="str">
         <f>Backlog!B8</f>
         <v>US12</v>
@@ -7710,7 +7738,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" customHeight="1">
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>301</v>
       </c>
@@ -7725,7 +7753,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="40"/>
     </row>
-    <row r="30" spans="1:9" ht="15" customHeight="1">
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>303</v>
       </c>
@@ -7740,7 +7768,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="40"/>
     </row>
-    <row r="31" spans="1:9" ht="15" customHeight="1">
+    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>305</v>
       </c>
@@ -7755,7 +7783,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="40"/>
     </row>
-    <row r="32" spans="1:9" ht="25.5" customHeight="1">
+    <row r="32" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>139</v>
       </c>
@@ -7770,7 +7798,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" spans="1:256" ht="25.5" customHeight="1">
+    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>141</v>
       </c>
@@ -7785,7 +7813,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:256" ht="15" customHeight="1">
+    <row r="34" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="7"/>
       <c r="C34" s="3"/>
@@ -7796,7 +7824,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:256" ht="15" customHeight="1">
+    <row r="35" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="29" t="s">
         <v>265</v>
@@ -7815,7 +7843,7 @@
       </c>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:256" ht="15" customHeight="1">
+    <row r="36" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="29"/>
       <c r="C36" s="3"/>
@@ -7826,7 +7854,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:256" ht="15" customHeight="1">
+    <row r="37" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="29" t="s">
         <v>266</v>
@@ -7839,7 +7867,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:256" ht="25.5" customHeight="1">
+    <row r="38" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="7" t="s">
         <v>143</v>
@@ -7852,7 +7880,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:256" ht="63.75" customHeight="1">
+    <row r="39" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7" t="s">
         <v>144</v>
@@ -7865,7 +7893,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:256" ht="63.75" customHeight="1">
+    <row r="40" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="66" t="s">
         <v>52</v>
@@ -8125,7 +8153,7 @@
       <c r="IU40" s="44"/>
       <c r="IV40" s="44"/>
     </row>
-    <row r="41" spans="1:256" ht="59" customHeight="1">
+    <row r="41" spans="1:256" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="33" t="s">
         <v>24</v>
@@ -8138,7 +8166,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:256" ht="15" customHeight="1">
+    <row r="42" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="29" t="s">
         <v>119</v>
@@ -8151,7 +8179,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="1:256" ht="89.25" customHeight="1">
+    <row r="43" spans="1:256" ht="89.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="33" t="s">
         <v>63</v>
@@ -8164,7 +8192,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="1:256" ht="51" customHeight="1">
+    <row r="44" spans="1:256" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3"/>
       <c r="B44" s="33" t="s">
         <v>64</v>
@@ -8177,7 +8205,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="1:256" ht="63.75" customHeight="1">
+    <row r="45" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="B45" s="33" t="s">
         <v>65</v>
@@ -8190,7 +8218,7 @@
       <c r="H45" s="3"/>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="1:256" ht="63.75" customHeight="1">
+    <row r="46" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="B46" s="33" t="s">
         <v>23</v>
@@ -8450,7 +8478,7 @@
       <c r="IU46" s="44"/>
       <c r="IV46" s="44"/>
     </row>
-    <row r="47" spans="1:256" ht="63.75" customHeight="1">
+    <row r="47" spans="1:256" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="33" t="s">
         <v>53</v>
@@ -8711,36 +8739,30 @@
       <c r="IV47" s="44"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV44"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="41" customWidth="1"/>
     <col min="2" max="2" width="18" style="41" customWidth="1"/>
     <col min="3" max="256" width="11" style="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="25.5" customHeight="1">
+    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>292</v>
       </c>
@@ -8769,7 +8791,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:256" ht="15" customHeight="1">
+    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>155</v>
       </c>
@@ -8799,7 +8821,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="38.25" customHeight="1">
+    <row r="3" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
@@ -8816,7 +8838,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="25.5" customHeight="1">
+    <row r="4" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -8833,7 +8855,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:256" ht="25.5" customHeight="1">
+    <row r="5" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>71</v>
       </c>
@@ -8850,7 +8872,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:256" ht="15" customHeight="1">
+    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="33"/>
       <c r="C6" s="3"/>
@@ -8861,7 +8883,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:256" ht="15" customHeight="1">
+    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>158</v>
       </c>
@@ -8891,7 +8913,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:256" ht="25.5" customHeight="1">
+    <row r="8" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
@@ -8906,7 +8928,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:256" ht="38.25" customHeight="1">
+    <row r="9" spans="1:256" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>180</v>
       </c>
@@ -8921,7 +8943,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:256" ht="25.5" customHeight="1">
+    <row r="10" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>182</v>
       </c>
@@ -8936,7 +8958,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:256" ht="25.5" customHeight="1">
+    <row r="11" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="33"/>
       <c r="C11" s="3"/>
@@ -8947,7 +8969,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="25.5" customHeight="1">
+    <row r="12" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>160</v>
       </c>
@@ -8976,7 +8998,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="13" spans="1:256" ht="25.5" customHeight="1">
+    <row r="13" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>184</v>
       </c>
@@ -8991,7 +9013,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="25.5" customHeight="1">
+    <row r="14" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>186</v>
       </c>
@@ -9006,7 +9028,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="25.5" customHeight="1">
+    <row r="15" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="67" t="s">
         <v>54</v>
       </c>
@@ -9268,7 +9290,7 @@
       <c r="IU15" s="44"/>
       <c r="IV15" s="44"/>
     </row>
-    <row r="16" spans="1:256" ht="25.5" customHeight="1">
+    <row r="16" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="33"/>
       <c r="C16" s="3"/>
@@ -9279,7 +9301,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:256" ht="25.5" customHeight="1">
+    <row r="17" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>162</v>
       </c>
@@ -9308,7 +9330,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:256" ht="25.5" customHeight="1">
+    <row r="18" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>188</v>
       </c>
@@ -9323,7 +9345,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:256" ht="25.5" customHeight="1">
+    <row r="19" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>189</v>
       </c>
@@ -9338,7 +9360,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:256" ht="25.5" customHeight="1">
+    <row r="20" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="67" t="s">
         <v>55</v>
       </c>
@@ -9600,7 +9622,7 @@
       <c r="IU20" s="44"/>
       <c r="IV20" s="44"/>
     </row>
-    <row r="21" spans="1:256" ht="25.5" customHeight="1">
+    <row r="21" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="35"/>
       <c r="B21" s="33"/>
       <c r="C21" s="3"/>
@@ -9611,7 +9633,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:256" ht="25.5" customHeight="1">
+    <row r="22" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>164</v>
       </c>
@@ -9887,7 +9909,7 @@
       <c r="IU22" s="44"/>
       <c r="IV22" s="44"/>
     </row>
-    <row r="23" spans="1:256" ht="25.5" customHeight="1">
+    <row r="23" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>48</v>
       </c>
@@ -10149,7 +10171,7 @@
       <c r="IU23" s="44"/>
       <c r="IV23" s="44"/>
     </row>
-    <row r="24" spans="1:256" ht="25.5" customHeight="1">
+    <row r="24" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
@@ -10411,7 +10433,7 @@
       <c r="IU24" s="44"/>
       <c r="IV24" s="44"/>
     </row>
-    <row r="25" spans="1:256" ht="25.5" customHeight="1">
+    <row r="25" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="67" t="s">
         <v>56</v>
       </c>
@@ -10673,7 +10695,7 @@
       <c r="IU25" s="44"/>
       <c r="IV25" s="44"/>
     </row>
-    <row r="26" spans="1:256" ht="25.5" customHeight="1">
+    <row r="26" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2"/>
       <c r="B26" s="64"/>
       <c r="C26" s="3"/>
@@ -10931,7 +10953,7 @@
       <c r="IU26" s="44"/>
       <c r="IV26" s="44"/>
     </row>
-    <row r="27" spans="1:256" ht="25.5" customHeight="1">
+    <row r="27" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>166</v>
       </c>
@@ -11207,7 +11229,7 @@
       <c r="IU27" s="44"/>
       <c r="IV27" s="44"/>
     </row>
-    <row r="28" spans="1:256" ht="25.5" customHeight="1">
+    <row r="28" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
@@ -11469,7 +11491,7 @@
       <c r="IU28" s="44"/>
       <c r="IV28" s="44"/>
     </row>
-    <row r="29" spans="1:256" ht="25.5" customHeight="1">
+    <row r="29" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -11731,7 +11753,7 @@
       <c r="IU29" s="44"/>
       <c r="IV29" s="44"/>
     </row>
-    <row r="30" spans="1:256" ht="25.5" customHeight="1">
+    <row r="30" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
@@ -11993,7 +12015,7 @@
       <c r="IU30" s="44"/>
       <c r="IV30" s="44"/>
     </row>
-    <row r="31" spans="1:256" ht="25.5" customHeight="1">
+    <row r="31" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>39</v>
       </c>
@@ -12255,7 +12277,7 @@
       <c r="IU31" s="44"/>
       <c r="IV31" s="44"/>
     </row>
-    <row r="32" spans="1:256" ht="25.5" customHeight="1">
+    <row r="32" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="67" t="s">
         <v>57</v>
       </c>
@@ -12517,7 +12539,7 @@
       <c r="IU32" s="44"/>
       <c r="IV32" s="44"/>
     </row>
-    <row r="33" spans="1:256" ht="25.5" customHeight="1">
+    <row r="33" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2"/>
       <c r="B33" s="64"/>
       <c r="C33" s="3"/>
@@ -12775,7 +12797,7 @@
       <c r="IU33" s="44"/>
       <c r="IV33" s="44"/>
     </row>
-    <row r="34" spans="1:256" ht="12.75" customHeight="1">
+    <row r="34" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="71" t="s">
         <v>257</v>
       </c>
@@ -12794,7 +12816,7 @@
       </c>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:256" ht="12.75" customHeight="1">
+    <row r="35" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="69" t="s">
         <v>310</v>
@@ -12807,7 +12829,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:256" ht="12.75" customHeight="1">
+    <row r="36" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="69" t="s">
         <v>309</v>
@@ -13067,7 +13089,7 @@
       <c r="IU36" s="44"/>
       <c r="IV36" s="44"/>
     </row>
-    <row r="37" spans="1:256" ht="12.75" customHeight="1">
+    <row r="37" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="69" t="s">
         <v>313</v>
@@ -13327,7 +13349,7 @@
       <c r="IU37" s="44"/>
       <c r="IV37" s="44"/>
     </row>
-    <row r="38" spans="1:256" ht="12.75" customHeight="1">
+    <row r="38" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -13338,7 +13360,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:256" ht="12.75" customHeight="1">
+    <row r="39" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -13349,7 +13371,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:256" ht="12.75" customHeight="1">
+    <row r="40" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="71" t="s">
         <v>119</v>
       </c>
@@ -13362,7 +13384,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:256" ht="12.75" customHeight="1">
+    <row r="41" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="69" t="s">
         <v>311</v>
@@ -13375,7 +13397,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:256" ht="12.75" customHeight="1">
+    <row r="42" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="69" t="s">
         <v>312</v>
@@ -13635,7 +13657,7 @@
       <c r="IU42" s="44"/>
       <c r="IV42" s="44"/>
     </row>
-    <row r="43" spans="1:256" ht="12.75" customHeight="1">
+    <row r="43" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="65" t="s">
         <v>314</v>
@@ -13648,7 +13670,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:256" ht="12.75" customHeight="1">
+    <row r="44" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3"/>
       <c r="B44" s="65" t="s">
         <v>315</v>
@@ -13662,36 +13684,30 @@
       <c r="I44" s="3"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="42"/>
-    <col min="2" max="2" width="21.140625" style="42" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="42" customWidth="1"/>
     <col min="3" max="256" width="11" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="25.5" customHeight="1">
+    <row r="1" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>292</v>
       </c>
@@ -13720,7 +13736,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:256" ht="15" customHeight="1">
+    <row r="2" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="68" t="str">
         <f>Backlog!$B$17</f>
         <v>US28</v>
@@ -13745,7 +13761,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:256" ht="15" customHeight="1">
+    <row r="3" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
         <v>235</v>
       </c>
@@ -14007,7 +14023,7 @@
       <c r="IU3" s="44"/>
       <c r="IV3" s="44"/>
     </row>
-    <row r="4" spans="1:256" ht="15" customHeight="1">
+    <row r="4" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
         <v>236</v>
       </c>
@@ -14269,7 +14285,7 @@
       <c r="IU4" s="44"/>
       <c r="IV4" s="44"/>
     </row>
-    <row r="5" spans="1:256" ht="15" customHeight="1">
+    <row r="5" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
         <v>240</v>
       </c>
@@ -14531,7 +14547,7 @@
       <c r="IU5" s="44"/>
       <c r="IV5" s="44"/>
     </row>
-    <row r="6" spans="1:256" ht="15" customHeight="1">
+    <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="70"/>
       <c r="B6" s="70"/>
       <c r="C6" s="69"/>
@@ -14789,7 +14805,7 @@
       <c r="IU6" s="44"/>
       <c r="IV6" s="44"/>
     </row>
-    <row r="7" spans="1:256" ht="15" customHeight="1">
+    <row r="7" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="68" t="str">
         <f>Backlog!$B$18</f>
         <v>US30</v>
@@ -14814,7 +14830,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:256" ht="15" customHeight="1">
+    <row r="8" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="69" t="s">
         <v>239</v>
       </c>
@@ -14829,7 +14845,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:256" ht="15" customHeight="1">
+    <row r="9" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="69" t="s">
         <v>244</v>
       </c>
@@ -14844,7 +14860,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:256" ht="15" customHeight="1">
+    <row r="10" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="69" t="s">
         <v>245</v>
       </c>
@@ -14859,7 +14875,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:256" ht="15" customHeight="1">
+    <row r="11" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -14870,7 +14886,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="15" customHeight="1">
+    <row r="12" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="71" t="s">
         <v>172</v>
       </c>
@@ -14893,7 +14909,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:256" ht="15" customHeight="1">
+    <row r="13" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="69" t="s">
         <v>248</v>
       </c>
@@ -14908,7 +14924,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="15" customHeight="1">
+    <row r="14" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="69" t="s">
         <v>250</v>
       </c>
@@ -14923,7 +14939,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="12.75" customHeight="1">
+    <row r="15" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -14934,7 +14950,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:256" ht="12.75" customHeight="1">
+    <row r="16" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="71" t="s">
         <v>174</v>
       </c>
@@ -14957,7 +14973,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:256" ht="12.75" customHeight="1">
+    <row r="17" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="69" t="s">
         <v>251</v>
       </c>
@@ -14972,7 +14988,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:256" ht="12.75" customHeight="1">
+    <row r="18" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="69" t="s">
         <v>253</v>
       </c>
@@ -14987,7 +15003,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:256" ht="12.75" customHeight="1">
+    <row r="19" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="69" t="s">
         <v>255</v>
       </c>
@@ -15002,7 +15018,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:256" ht="12.75" customHeight="1">
+    <row r="20" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -15013,7 +15029,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:256" ht="12.75" customHeight="1">
+    <row r="21" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="71" t="s">
         <v>316</v>
       </c>
@@ -15023,8 +15039,8 @@
       <c r="C21" s="65" t="s">
         <v>319</v>
       </c>
-      <c r="D21" s="69" t="s">
-        <v>66</v>
+      <c r="D21" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="E21" s="3">
         <v>45</v>
@@ -15032,11 +15048,17 @@
       <c r="F21" s="3">
         <v>90</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:256" ht="12.75" customHeight="1">
+      <c r="G21" s="3">
+        <v>33</v>
+      </c>
+      <c r="H21" s="3">
+        <v>90</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="65" t="s">
         <v>321</v>
       </c>
@@ -15051,7 +15073,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:256" ht="12.75" customHeight="1">
+    <row r="23" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="65" t="s">
         <v>325</v>
       </c>
@@ -15066,7 +15088,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:256" ht="12.75" customHeight="1">
+    <row r="24" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="65" t="s">
         <v>327</v>
       </c>
@@ -15328,7 +15350,7 @@
       <c r="IU24" s="44"/>
       <c r="IV24" s="44"/>
     </row>
-    <row r="25" spans="1:256" ht="12.75" customHeight="1">
+    <row r="25" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="65" t="s">
         <v>329</v>
       </c>
@@ -15590,7 +15612,7 @@
       <c r="IU25" s="44"/>
       <c r="IV25" s="44"/>
     </row>
-    <row r="26" spans="1:256" ht="12.75" customHeight="1">
+    <row r="26" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -15601,7 +15623,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:256" ht="12.75" customHeight="1">
+    <row r="27" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="71" t="s">
         <v>317</v>
       </c>
@@ -15611,8 +15633,8 @@
       <c r="C27" s="65" t="s">
         <v>320</v>
       </c>
-      <c r="D27" s="69" t="s">
-        <v>66</v>
+      <c r="D27" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="E27" s="3">
         <v>30</v>
@@ -15620,11 +15642,17 @@
       <c r="F27" s="3">
         <v>60</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:256" ht="12.75" customHeight="1">
+      <c r="G27" s="3">
+        <v>12</v>
+      </c>
+      <c r="H27" s="3">
+        <v>30</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="65" t="s">
         <v>323</v>
       </c>
@@ -15639,7 +15667,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:256" ht="12.75" customHeight="1">
+    <row r="29" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="65" t="s">
         <v>330</v>
       </c>
@@ -15654,7 +15682,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:256" ht="12.75" customHeight="1">
+    <row r="30" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="65" t="s">
         <v>330</v>
       </c>
@@ -15669,7 +15697,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:256" ht="12.75" customHeight="1">
+    <row r="31" spans="1:256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -15681,33 +15709,28 @@
       <c r="I31" s="3"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="9" width="11" style="43" customWidth="1"/>
     <col min="10" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" customHeight="1">
+    <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>292</v>
       </c>
@@ -15736,7 +15759,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -15747,7 +15770,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -15758,7 +15781,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -15769,7 +15792,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -15780,7 +15803,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -15791,7 +15814,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -15802,7 +15825,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -15813,7 +15836,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -15824,7 +15847,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -15836,16 +15859,10 @@
       <c r="I10" s="3"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>